<commit_message>
changed IPT adherence to not differentiate between genders
</commit_message>
<xml_diff>
--- a/param_files/Epi_model_parameters.xlsx
+++ b/param_files/Epi_model_parameters.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10810"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chelseagreene/ws/github/ws.epi_model_HIV_TB/epi_model_HIV_TB/param_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C44E8778-1567-D846-AB69-DD88740F21CF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C96B570A-E970-4D45-AD19-CD936B1E7D14}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-33480" yWindow="3940" windowWidth="30260" windowHeight="17160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -137,7 +137,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1124" uniqueCount="368">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1115" uniqueCount="366">
   <si>
     <t>Epidemiological data point (description)</t>
   </si>
@@ -1225,22 +1225,16 @@
     <t>varpi</t>
   </si>
   <si>
-    <t>IPT Adherence for gender compartment Male under policy Community ART</t>
-  </si>
-  <si>
-    <t>IPT Adherence for gender compartment Female under policy Community ART</t>
-  </si>
-  <si>
-    <t>IPT Adherence for gender compartment Male under policy Standard (baseline)</t>
-  </si>
-  <si>
-    <t>IPT Adherence for gender compartment Female under policy Standard (baseline)</t>
-  </si>
-  <si>
     <t xml:space="preserve">Percentage HIV - </t>
   </si>
   <si>
     <t>Reference-Expected Value</t>
+  </si>
+  <si>
+    <t>IPT Adherence  under policy Community ART</t>
+  </si>
+  <si>
+    <t>IPT Adherence  under policy Standard (baseline)</t>
   </si>
 </sst>
 </file>
@@ -1807,13 +1801,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O195"/>
+  <dimension ref="A1:O192"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="10" ySplit="1" topLeftCell="K172" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="10" ySplit="1" topLeftCell="K180" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="I1" sqref="I1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="M173" sqref="M173"/>
+      <selection pane="bottomRight" activeCell="K190" sqref="K190"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -8349,7 +8343,7 @@
         <v>2</v>
       </c>
       <c r="J189" s="9" t="str">
-        <f t="shared" ref="J189:J195" si="20">CONCATENATE(C189, "_", E189, IF(E189&lt;&gt;"",",",""), F189, IF(F189&lt;&gt;"",",",""),  G189, IF(G189&lt;&gt;"",",",""),  H189, IF(I189&lt;&gt;"","(",""), I189, IF(I189&lt;&gt;"",")",""))</f>
+        <f t="shared" ref="J189:J192" si="20">CONCATENATE(C189, "_", E189, IF(E189&lt;&gt;"",",",""), F189, IF(F189&lt;&gt;"",",",""),  G189, IF(G189&lt;&gt;"",",",""),  H189, IF(I189&lt;&gt;"","(",""), I189, IF(I189&lt;&gt;"",")",""))</f>
         <v>rho_6,2,2</v>
       </c>
       <c r="K189" s="23">
@@ -8359,11 +8353,11 @@
     </row>
     <row r="190" spans="1:11" ht="32">
       <c r="A190" s="11" t="s">
-        <v>362</v>
+        <v>364</v>
       </c>
       <c r="B190" s="9" t="str">
-        <f>CONCATENATE("IPT Adherence for gender compartment ", VLOOKUP(H190, G_SET, 2),  " under policy ", VLOOKUP(I60, P_SET,2))</f>
-        <v>IPT Adherence for gender compartment Male under policy Community ART</v>
+        <f>CONCATENATE("IPT Adherence  under policy ", VLOOKUP(I60, P_SET,2))</f>
+        <v>IPT Adherence  under policy Community ART</v>
       </c>
       <c r="C190" s="9" t="s">
         <v>361</v>
@@ -8371,15 +8365,12 @@
       <c r="D190" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="H190" s="9">
-        <v>1</v>
-      </c>
       <c r="I190" s="9">
         <v>1</v>
       </c>
       <c r="J190" s="9" t="str">
         <f t="shared" si="20"/>
-        <v>varpi_1(1)</v>
+        <v>varpi_(1)</v>
       </c>
       <c r="K190" s="35">
         <v>0.2</v>
@@ -8387,11 +8378,11 @@
     </row>
     <row r="191" spans="1:11" ht="32">
       <c r="A191" s="11" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="B191" s="9" t="str">
-        <f>CONCATENATE("IPT Adherence for gender compartment ", VLOOKUP(H191, G_SET, 2),  " under policy ", VLOOKUP(I61, P_SET,2))</f>
-        <v>IPT Adherence for gender compartment Female under policy Community ART</v>
+        <f>CONCATENATE("IPT Adherence  under policy ", VLOOKUP(I61, P_SET,2))</f>
+        <v>IPT Adherence  under policy Community ART</v>
       </c>
       <c r="C191" s="9" t="s">
         <v>361</v>
@@ -8399,15 +8390,12 @@
       <c r="D191" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="H191" s="9">
-        <v>2</v>
-      </c>
       <c r="I191" s="9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J191" s="9" t="str">
         <f t="shared" si="20"/>
-        <v>varpi_2(1)</v>
+        <v>varpi_(2)</v>
       </c>
       <c r="K191" s="35">
         <v>0.2</v>
@@ -8415,11 +8403,11 @@
     </row>
     <row r="192" spans="1:11" ht="32">
       <c r="A192" s="11" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="B192" s="9" t="str">
-        <f>CONCATENATE("IPT Adherence for gender compartment ", VLOOKUP(H192, G_SET, 2),  " under policy ", VLOOKUP(I62, P_SET,2))</f>
-        <v>IPT Adherence for gender compartment Male under policy Standard (baseline)</v>
+        <f>CONCATENATE("IPT Adherence  under policy ", VLOOKUP(I62, P_SET,2))</f>
+        <v>IPT Adherence  under policy Standard (baseline)</v>
       </c>
       <c r="C192" s="9" t="s">
         <v>361</v>
@@ -8427,101 +8415,14 @@
       <c r="D192" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="H192" s="9">
-        <v>1</v>
-      </c>
       <c r="I192" s="9">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J192" s="9" t="str">
         <f t="shared" si="20"/>
-        <v>varpi_1(2)</v>
+        <v>varpi_(3)</v>
       </c>
       <c r="K192" s="35">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="193" spans="1:11" ht="32">
-      <c r="A193" s="11" t="s">
-        <v>365</v>
-      </c>
-      <c r="B193" s="9" t="str">
-        <f>CONCATENATE("IPT Adherence for gender compartment ", VLOOKUP(H193, G_SET, 2),  " under policy ", VLOOKUP(I63, P_SET,2))</f>
-        <v>IPT Adherence for gender compartment Female under policy Standard (baseline)</v>
-      </c>
-      <c r="C193" s="9" t="s">
-        <v>361</v>
-      </c>
-      <c r="D193" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="H193" s="9">
-        <v>2</v>
-      </c>
-      <c r="I193" s="9">
-        <v>2</v>
-      </c>
-      <c r="J193" s="9" t="str">
-        <f t="shared" si="20"/>
-        <v>varpi_2(2)</v>
-      </c>
-      <c r="K193" s="35">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="194" spans="1:11" ht="32">
-      <c r="A194" s="11" t="s">
-        <v>364</v>
-      </c>
-      <c r="B194" s="9" t="str">
-        <f>CONCATENATE("IPT Adherence for gender compartment ", VLOOKUP(H194, G_SET, 2),  " under policy ", VLOOKUP(I64, P_SET,2))</f>
-        <v>IPT Adherence for gender compartment Male under policy Standard (baseline)</v>
-      </c>
-      <c r="C194" s="9" t="s">
-        <v>361</v>
-      </c>
-      <c r="D194" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="H194" s="9">
-        <v>1</v>
-      </c>
-      <c r="I194" s="9">
-        <v>3</v>
-      </c>
-      <c r="J194" s="9" t="str">
-        <f t="shared" si="20"/>
-        <v>varpi_1(3)</v>
-      </c>
-      <c r="K194" s="35">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="195" spans="1:11" ht="32">
-      <c r="A195" s="11" t="s">
-        <v>365</v>
-      </c>
-      <c r="B195" s="9" t="str">
-        <f>CONCATENATE("IPT Adherence for gender compartment ", VLOOKUP(H195, G_SET, 2),  " under policy ", VLOOKUP(I65, P_SET,2))</f>
-        <v>IPT Adherence for gender compartment Female under policy Standard (baseline)</v>
-      </c>
-      <c r="C195" s="9" t="s">
-        <v>361</v>
-      </c>
-      <c r="D195" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="H195" s="9">
-        <v>2</v>
-      </c>
-      <c r="I195" s="9">
-        <v>3</v>
-      </c>
-      <c r="J195" s="9" t="str">
-        <f t="shared" si="20"/>
-        <v>varpi_2(3)</v>
-      </c>
-      <c r="K195" s="35">
         <v>0.8</v>
       </c>
     </row>
@@ -8862,7 +8763,7 @@
     </row>
     <row r="17" spans="1:13" ht="17">
       <c r="A17" s="37" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="B17" s="32"/>
       <c r="C17" s="32"/>
@@ -10149,7 +10050,7 @@
         <v>328</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="O1" s="16" t="s">
         <v>11</v>

</xml_diff>

<commit_message>
calibration run april 25th
</commit_message>
<xml_diff>
--- a/param_files/Epi_model_parameters.xlsx
+++ b/param_files/Epi_model_parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10323"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chelseagreene/github/epi_model_HIV_TB/param_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F411C6B1-4D70-8349-8AFC-A8B14B76021B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33411958-7E7A-5C49-96C5-A73AF157F611}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13180" yWindow="620" windowWidth="35840" windowHeight="20200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="model_matched_parameters" sheetId="1" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1650" uniqueCount="641">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1650" uniqueCount="639">
   <si>
     <t>Epidemiological data point (description)</t>
   </si>
@@ -1903,9 +1903,6 @@
   </si>
   <si>
     <t>Jen agrees, but question for timing. Does this all happen in one year?-- CG note 91% initiation, 75% adherence</t>
-  </si>
-  <si>
-    <t>cg: set to 50% reduction of average of recent and remote rate</t>
   </si>
   <si>
     <t>xi</t>
@@ -2008,9 +2005,6 @@
       </rPr>
       <t> 104.5 (2014).</t>
     </r>
-  </si>
-  <si>
-    <t>cg: set to 70% reduction of average of recent and remote rate</t>
   </si>
   <si>
     <t>Jenn Ref</t>
@@ -2792,10 +2786,10 @@
   <dimension ref="A1:Q224"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="119" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="11" ySplit="1" topLeftCell="L2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="11" ySplit="1" topLeftCell="L88" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="I1" sqref="I1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L9" sqref="L9"/>
+      <selection pane="bottomRight" activeCell="P97" sqref="P97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3170,7 +3164,7 @@
     </row>
     <row r="10" spans="1:17" ht="51" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="61" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="B10" s="21"/>
       <c r="C10" s="8" t="s">
@@ -3188,23 +3182,23 @@
         <v>upsilon_1,</v>
       </c>
       <c r="K10" s="9" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="L10" s="9">
         <f>0.5</f>
         <v>0.5</v>
       </c>
       <c r="O10" s="62" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="P10" s="41" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="Q10" s="42"/>
     </row>
     <row r="11" spans="1:17" ht="51" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="61" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="B11" s="21"/>
       <c r="C11" s="8" t="s">
@@ -3222,22 +3216,22 @@
         <v>upsilon_2,</v>
       </c>
       <c r="K11" s="9" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="L11" s="9">
         <v>1</v>
       </c>
       <c r="O11" s="62" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="P11" s="41" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="Q11" s="42"/>
     </row>
     <row r="12" spans="1:17" ht="51" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="61" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="B12" s="21"/>
       <c r="C12" s="8" t="s">
@@ -3255,22 +3249,22 @@
         <v>upsilon_3,</v>
       </c>
       <c r="K12" s="9" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="L12" s="9">
         <v>1</v>
       </c>
       <c r="O12" s="62" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="P12" s="41" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="Q12" s="42"/>
     </row>
     <row r="13" spans="1:17" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="61" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="B13" s="21"/>
       <c r="C13" s="8" t="s">
@@ -3288,26 +3282,26 @@
         <v>upsilon_4,</v>
       </c>
       <c r="K13" s="9" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="L13" s="9">
         <v>1</v>
       </c>
       <c r="O13" s="40" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="P13" s="41" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="Q13" s="42"/>
     </row>
     <row r="14" spans="1:17" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="63" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="B14" s="21"/>
       <c r="C14" s="8" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="D14" s="8" t="s">
         <v>38</v>
@@ -3318,16 +3312,16 @@
         <v>xi_</v>
       </c>
       <c r="K14" s="9" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="L14" s="23">
         <v>4</v>
       </c>
       <c r="O14" s="64" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="P14" s="40" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="Q14" s="42"/>
     </row>
@@ -6916,7 +6910,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="96" spans="1:17" ht="32" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A96" s="20" t="s">
         <v>127</v>
       </c>
@@ -6940,12 +6934,12 @@
         <v>445</v>
       </c>
       <c r="L96" s="23">
-        <f>AVERAGE(L94,L95)*0.3</f>
-        <v>7.6500000000000005E-3</v>
+        <f>0.0075</f>
+        <v>7.4999999999999997E-3</v>
       </c>
       <c r="O96" s="40"/>
       <c r="P96" s="41" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="Q96" s="42" t="s">
         <v>315</v>
@@ -6978,10 +6972,10 @@
         <v>8.0000000000000002E-3</v>
       </c>
       <c r="O97" s="9" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
       <c r="P97" s="41" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="Q97" s="10" t="s">
         <v>314</v>
@@ -7014,10 +7008,10 @@
         <v>2</v>
       </c>
       <c r="O98" s="65" t="s">
+        <v>636</v>
+      </c>
+      <c r="P98" s="66" t="s">
         <v>637</v>
-      </c>
-      <c r="P98" s="66" t="s">
-        <v>638</v>
       </c>
       <c r="Q98" s="42" t="s">
         <v>315</v>
@@ -7045,12 +7039,12 @@
         <v>610</v>
       </c>
       <c r="L99" s="23">
-        <f>AVERAGE(L94,L95)*0.5</f>
-        <v>1.2750000000000001E-2</v>
+        <f>0.0038</f>
+        <v>3.8E-3</v>
       </c>
       <c r="O99" s="40"/>
       <c r="P99" s="41" t="s">
-        <v>618</v>
+        <v>638</v>
       </c>
       <c r="Q99" s="42"/>
     </row>

</xml_diff>

<commit_message>
calibration before running 6-10 betas
</commit_message>
<xml_diff>
--- a/param_files/Epi_model_parameters.xlsx
+++ b/param_files/Epi_model_parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chelseagreene/github/epi_model_HIV_TB/param_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC86193A-68ED-3E49-8937-AB398AA80125}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C83021EA-5363-A345-A1D5-51C8F892AF86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="35840" windowHeight="20560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="model_matched_parameters" sheetId="1" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1653" uniqueCount="639">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1652" uniqueCount="638">
   <si>
     <t>Epidemiological data point (description)</t>
   </si>
@@ -1927,12 +1927,6 @@
   </si>
   <si>
     <t>upsilon_4,</t>
-  </si>
-  <si>
-    <t>Total time between 6-&gt;7 = 1 year (6 months to initiate treatment, 6 months of treatment), so to double rate .5</t>
-  </si>
-  <si>
-    <t>Assume diagnosed right away</t>
   </si>
   <si>
     <t>https://www.atsjournals.org/doi/pdf/10.1164/rccm.201111-1941OC</t>
@@ -1977,9 +1971,6 @@
     <t>https://journals.lww.com/aidsonline/fulltext/1999/08200/relapse_and_mortality_among_hiv_infected_and.15.aspx?casa_token=vWxO6_8KJzUAAAAA:ZO9CgaeDwvG-EClLVdnyIZJcVy6hs5FXUKMwwttTiELpLxc9Z7Mm25A76myj-SVbN_kQ9sIvz5levVDOFQhBRMSf</t>
   </si>
   <si>
-    <t>Should we include adherence?</t>
-  </si>
-  <si>
     <r>
       <t>Ershova, Julia V., et al. "Evaluation of adherence to national treatment guidelines among tuberculosis patients in three provinces of South Africa." </t>
     </r>
@@ -2008,6 +1999,12 @@
   </si>
   <si>
     <t>Changed to Jenn Ref</t>
+  </si>
+  <si>
+    <t>Total time between 6-&gt;7 = 1.5 year (6 months to initiate treatment, 6 months of treatment), so x1/3</t>
+  </si>
+  <si>
+    <t>Assume 1 year active</t>
   </si>
 </sst>
 </file>
@@ -2786,10 +2783,10 @@
   <dimension ref="A1:Q224"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="119" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="11" ySplit="1" topLeftCell="L93" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="11" ySplit="1" topLeftCell="L95" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="I1" sqref="I1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="O101" sqref="O101"/>
+      <selection pane="bottomRight" activeCell="O98" sqref="O98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3185,14 +3182,14 @@
         <v>622</v>
       </c>
       <c r="L10" s="9">
-        <f>0.5</f>
-        <v>0.5</v>
+        <f>1/3</f>
+        <v>0.33333333333333331</v>
       </c>
       <c r="O10" s="61" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
       <c r="P10" s="40" t="s">
-        <v>626</v>
+        <v>636</v>
       </c>
       <c r="Q10" s="41"/>
     </row>
@@ -3219,13 +3216,14 @@
         <v>623</v>
       </c>
       <c r="L11" s="9">
-        <v>1</v>
+        <f t="shared" ref="L11:L13" si="1">0.5</f>
+        <v>0.5</v>
       </c>
       <c r="O11" s="61" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
       <c r="P11" s="40" t="s">
-        <v>627</v>
+        <v>637</v>
       </c>
       <c r="Q11" s="41"/>
     </row>
@@ -3252,13 +3250,14 @@
         <v>624</v>
       </c>
       <c r="L12" s="9">
-        <v>1</v>
+        <f t="shared" si="1"/>
+        <v>0.5</v>
       </c>
       <c r="O12" s="61" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
       <c r="P12" s="40" t="s">
-        <v>627</v>
+        <v>637</v>
       </c>
       <c r="Q12" s="41"/>
     </row>
@@ -3285,19 +3284,20 @@
         <v>625</v>
       </c>
       <c r="L13" s="9">
-        <v>1</v>
+        <f t="shared" si="1"/>
+        <v>0.5</v>
       </c>
       <c r="O13" s="39" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
       <c r="P13" s="40" t="s">
-        <v>627</v>
+        <v>637</v>
       </c>
       <c r="Q13" s="41"/>
     </row>
     <row r="14" spans="1:17" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="62" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
       <c r="B14" s="21"/>
       <c r="C14" s="8" t="s">
@@ -3312,16 +3312,16 @@
         <v>xi_</v>
       </c>
       <c r="K14" s="9" t="s">
-        <v>632</v>
+        <v>630</v>
       </c>
       <c r="L14" s="23">
         <v>4</v>
       </c>
       <c r="O14" s="63" t="s">
+        <v>629</v>
+      </c>
+      <c r="P14" s="39" t="s">
         <v>631</v>
-      </c>
-      <c r="P14" s="39" t="s">
-        <v>633</v>
       </c>
       <c r="Q14" s="41"/>
     </row>
@@ -3502,7 +3502,7 @@
         <v>93</v>
       </c>
       <c r="B20" s="21" t="str">
-        <f t="shared" ref="B20:B51" si="1">CONCATENATE("Rate of IPT initiation from TB compartment ",VLOOKUP(E20,TB_SET,2)," and HIV compartment ",VLOOKUP(G20,HIV_SET,2)," for gender ",VLOOKUP(H20,G_SET,2), " under policy ", VLOOKUP(I20, P_SET,2))</f>
+        <f t="shared" ref="B20:B51" si="2">CONCATENATE("Rate of IPT initiation from TB compartment ",VLOOKUP(E20,TB_SET,2)," and HIV compartment ",VLOOKUP(G20,HIV_SET,2)," for gender ",VLOOKUP(H20,G_SET,2), " under policy ", VLOOKUP(I20, P_SET,2))</f>
         <v>Rate of IPT initiation from TB compartment  Uninfected, not on IPT and HIV compartment  HIV-negative for gender Male under policy Standard (baseline)</v>
       </c>
       <c r="C20" s="8" t="s">
@@ -3546,7 +3546,7 @@
         <v>94</v>
       </c>
       <c r="B21" s="21" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Rate of IPT initiation from TB compartment  Uninfected, not on IPT and HIV compartment  HIV-negative for gender Female under policy Standard (baseline)</v>
       </c>
       <c r="C21" s="8" t="s">
@@ -3590,7 +3590,7 @@
         <v>101</v>
       </c>
       <c r="B22" s="21" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Rate of IPT initiation from TB compartment  LTBI, infected recently (at risk for rapid progression) and HIV compartment  HIV-negative for gender Male under policy Standard (baseline)</v>
       </c>
       <c r="C22" s="8" t="s">
@@ -3634,7 +3634,7 @@
         <v>102</v>
       </c>
       <c r="B23" s="21" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Rate of IPT initiation from TB compartment  LTBI, infected recently (at risk for rapid progression) and HIV compartment  HIV-negative for gender Female under policy Standard (baseline)</v>
       </c>
       <c r="C23" s="8" t="s">
@@ -3678,7 +3678,7 @@
         <v>109</v>
       </c>
       <c r="B24" s="21" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Rate of IPT initiation from TB compartment  LTBI, infected remotely and HIV compartment  HIV-negative for gender Male under policy Standard (baseline)</v>
       </c>
       <c r="C24" s="8" t="s">
@@ -3722,7 +3722,7 @@
         <v>110</v>
       </c>
       <c r="B25" s="21" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Rate of IPT initiation from TB compartment  LTBI, infected remotely and HIV compartment  HIV-negative for gender Female under policy Standard (baseline)</v>
       </c>
       <c r="C25" s="8" t="s">
@@ -3766,7 +3766,7 @@
         <v>66</v>
       </c>
       <c r="B26" s="21" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Rate of IPT initiation from TB compartment  Uninfected, not on IPT and HIV compartment  HIV-negative for gender Male under policy Community ART</v>
       </c>
       <c r="C26" s="8" t="s">
@@ -3810,7 +3810,7 @@
         <v>68</v>
       </c>
       <c r="B27" s="21" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Rate of IPT initiation from TB compartment  Uninfected, not on IPT and HIV compartment  HIV-negative for gender Female under policy Community ART</v>
       </c>
       <c r="C27" s="8" t="s">
@@ -3854,7 +3854,7 @@
         <v>76</v>
       </c>
       <c r="B28" s="21" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Rate of IPT initiation from TB compartment  LTBI, infected recently (at risk for rapid progression) and HIV compartment  HIV-negative for gender Male under policy Community ART</v>
       </c>
       <c r="C28" s="8" t="s">
@@ -3898,7 +3898,7 @@
         <v>77</v>
       </c>
       <c r="B29" s="21" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Rate of IPT initiation from TB compartment  LTBI, infected recently (at risk for rapid progression) and HIV compartment  HIV-negative for gender Female under policy Community ART</v>
       </c>
       <c r="C29" s="8" t="s">
@@ -3942,7 +3942,7 @@
         <v>84</v>
       </c>
       <c r="B30" s="21" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Rate of IPT initiation from TB compartment  LTBI, infected remotely and HIV compartment  HIV-negative for gender Male under policy Community ART</v>
       </c>
       <c r="C30" s="8" t="s">
@@ -3986,7 +3986,7 @@
         <v>86</v>
       </c>
       <c r="B31" s="21" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Rate of IPT initiation from TB compartment  LTBI, infected remotely and HIV compartment  HIV-negative for gender Female under policy Community ART</v>
       </c>
       <c r="C31" s="8" t="s">
@@ -4030,7 +4030,7 @@
         <v>36</v>
       </c>
       <c r="B32" s="21" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Rate of IPT initiation from TB compartment  Uninfected, not on IPT and HIV compartment  HIV-negative for gender Male under policy Community ART + IPT</v>
       </c>
       <c r="C32" s="8" t="s">
@@ -4074,7 +4074,7 @@
         <v>40</v>
       </c>
       <c r="B33" s="21" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Rate of IPT initiation from TB compartment  Uninfected, not on IPT and HIV compartment  HIV-negative for gender Female under policy Community ART + IPT</v>
       </c>
       <c r="C33" s="8" t="s">
@@ -4118,7 +4118,7 @@
         <v>49</v>
       </c>
       <c r="B34" s="21" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Rate of IPT initiation from TB compartment  LTBI, infected recently (at risk for rapid progression) and HIV compartment  HIV-negative for gender Male under policy Community ART + IPT</v>
       </c>
       <c r="C34" s="8" t="s">
@@ -4162,7 +4162,7 @@
         <v>50</v>
       </c>
       <c r="B35" s="21" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Rate of IPT initiation from TB compartment  LTBI, infected recently (at risk for rapid progression) and HIV compartment  HIV-negative for gender Female under policy Community ART + IPT</v>
       </c>
       <c r="C35" s="8" t="s">
@@ -4206,7 +4206,7 @@
         <v>58</v>
       </c>
       <c r="B36" s="21" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Rate of IPT initiation from TB compartment  LTBI, infected remotely and HIV compartment  HIV-negative for gender Male under policy Community ART + IPT</v>
       </c>
       <c r="C36" s="8" t="s">
@@ -4250,7 +4250,7 @@
         <v>59</v>
       </c>
       <c r="B37" s="21" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Rate of IPT initiation from TB compartment  LTBI, infected remotely and HIV compartment  HIV-negative for gender Female under policy Community ART + IPT</v>
       </c>
       <c r="C37" s="8" t="s">
@@ -4294,7 +4294,7 @@
         <v>95</v>
       </c>
       <c r="B38" s="21" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Rate of IPT initiation from TB compartment  Uninfected, not on IPT and HIV compartment  PLHIV not on ART, CD4&gt;200 for gender Male under policy Standard (baseline)</v>
       </c>
       <c r="C38" s="8" t="s">
@@ -4323,7 +4323,7 @@
         <v>374</v>
       </c>
       <c r="L38" s="9">
-        <f t="shared" ref="L38:L49" si="2">0.06*0.06</f>
+        <f t="shared" ref="L38:L49" si="3">0.06*0.06</f>
         <v>3.5999999999999999E-3</v>
       </c>
       <c r="O38" s="39" t="s">
@@ -4341,7 +4341,7 @@
         <v>96</v>
       </c>
       <c r="B39" s="21" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Rate of IPT initiation from TB compartment  Uninfected, not on IPT and HIV compartment  PLHIV not on ART, CD4&gt;200 for gender Female under policy Standard (baseline)</v>
       </c>
       <c r="C39" s="8" t="s">
@@ -4370,7 +4370,7 @@
         <v>377</v>
       </c>
       <c r="L39" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3.5999999999999999E-3</v>
       </c>
       <c r="O39" s="39" t="s">
@@ -4388,7 +4388,7 @@
         <v>103</v>
       </c>
       <c r="B40" s="21" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Rate of IPT initiation from TB compartment  LTBI, infected recently (at risk for rapid progression) and HIV compartment  PLHIV not on ART, CD4&gt;200 for gender Male under policy Standard (baseline)</v>
       </c>
       <c r="C40" s="8" t="s">
@@ -4417,7 +4417,7 @@
         <v>398</v>
       </c>
       <c r="L40" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3.5999999999999999E-3</v>
       </c>
       <c r="O40" s="39" t="s">
@@ -4435,7 +4435,7 @@
         <v>104</v>
       </c>
       <c r="B41" s="21" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Rate of IPT initiation from TB compartment  LTBI, infected recently (at risk for rapid progression) and HIV compartment  PLHIV not on ART, CD4&gt;200 for gender Female under policy Standard (baseline)</v>
       </c>
       <c r="C41" s="8" t="s">
@@ -4464,7 +4464,7 @@
         <v>401</v>
       </c>
       <c r="L41" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3.5999999999999999E-3</v>
       </c>
       <c r="O41" s="39" t="s">
@@ -4482,7 +4482,7 @@
         <v>111</v>
       </c>
       <c r="B42" s="21" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Rate of IPT initiation from TB compartment  LTBI, infected remotely and HIV compartment  PLHIV not on ART, CD4&gt;200 for gender Male under policy Standard (baseline)</v>
       </c>
       <c r="C42" s="8" t="s">
@@ -4511,7 +4511,7 @@
         <v>422</v>
       </c>
       <c r="L42" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3.5999999999999999E-3</v>
       </c>
       <c r="O42" s="39" t="s">
@@ -4529,7 +4529,7 @@
         <v>112</v>
       </c>
       <c r="B43" s="21" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Rate of IPT initiation from TB compartment  LTBI, infected remotely and HIV compartment  PLHIV not on ART, CD4&gt;200 for gender Female under policy Standard (baseline)</v>
       </c>
       <c r="C43" s="8" t="s">
@@ -4558,7 +4558,7 @@
         <v>425</v>
       </c>
       <c r="L43" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3.5999999999999999E-3</v>
       </c>
       <c r="O43" s="39" t="s">
@@ -4576,7 +4576,7 @@
         <v>69</v>
       </c>
       <c r="B44" s="21" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Rate of IPT initiation from TB compartment  Uninfected, not on IPT and HIV compartment  PLHIV not on ART, CD4&gt;200 for gender Male under policy Community ART</v>
       </c>
       <c r="C44" s="8" t="s">
@@ -4605,7 +4605,7 @@
         <v>375</v>
       </c>
       <c r="L44" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3.5999999999999999E-3</v>
       </c>
       <c r="O44" s="39" t="s">
@@ -4623,7 +4623,7 @@
         <v>71</v>
       </c>
       <c r="B45" s="21" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Rate of IPT initiation from TB compartment  Uninfected, not on IPT and HIV compartment  PLHIV not on ART, CD4&gt;200 for gender Female under policy Community ART</v>
       </c>
       <c r="C45" s="8" t="s">
@@ -4652,7 +4652,7 @@
         <v>378</v>
       </c>
       <c r="L45" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3.5999999999999999E-3</v>
       </c>
       <c r="O45" s="39" t="s">
@@ -4670,7 +4670,7 @@
         <v>78</v>
       </c>
       <c r="B46" s="21" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Rate of IPT initiation from TB compartment  LTBI, infected recently (at risk for rapid progression) and HIV compartment  PLHIV not on ART, CD4&gt;200 for gender Male under policy Community ART</v>
       </c>
       <c r="C46" s="8" t="s">
@@ -4699,7 +4699,7 @@
         <v>399</v>
       </c>
       <c r="L46" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3.5999999999999999E-3</v>
       </c>
       <c r="O46" s="39" t="s">
@@ -4717,7 +4717,7 @@
         <v>79</v>
       </c>
       <c r="B47" s="21" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Rate of IPT initiation from TB compartment  LTBI, infected recently (at risk for rapid progression) and HIV compartment  PLHIV not on ART, CD4&gt;200 for gender Female under policy Community ART</v>
       </c>
       <c r="C47" s="8" t="s">
@@ -4746,7 +4746,7 @@
         <v>402</v>
       </c>
       <c r="L47" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3.5999999999999999E-3</v>
       </c>
       <c r="O47" s="39" t="s">
@@ -4764,7 +4764,7 @@
         <v>87</v>
       </c>
       <c r="B48" s="21" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Rate of IPT initiation from TB compartment  LTBI, infected remotely and HIV compartment  PLHIV not on ART, CD4&gt;200 for gender Male under policy Community ART</v>
       </c>
       <c r="C48" s="8" t="s">
@@ -4793,7 +4793,7 @@
         <v>423</v>
       </c>
       <c r="L48" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3.5999999999999999E-3</v>
       </c>
       <c r="O48" s="39" t="s">
@@ -4811,7 +4811,7 @@
         <v>88</v>
       </c>
       <c r="B49" s="21" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Rate of IPT initiation from TB compartment  LTBI, infected remotely and HIV compartment  PLHIV not on ART, CD4&gt;200 for gender Female under policy Community ART</v>
       </c>
       <c r="C49" s="8" t="s">
@@ -4840,7 +4840,7 @@
         <v>426</v>
       </c>
       <c r="L49" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3.5999999999999999E-3</v>
       </c>
       <c r="O49" s="39" t="s">
@@ -4858,7 +4858,7 @@
         <v>41</v>
       </c>
       <c r="B50" s="21" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Rate of IPT initiation from TB compartment  Uninfected, not on IPT and HIV compartment  PLHIV not on ART, CD4&gt;200 for gender Male under policy Community ART + IPT</v>
       </c>
       <c r="C50" s="8" t="s">
@@ -4887,7 +4887,7 @@
         <v>376</v>
       </c>
       <c r="L50" s="9">
-        <f t="shared" ref="L50:L55" si="3">0.91*0.75</f>
+        <f t="shared" ref="L50:L55" si="4">0.91*0.75</f>
         <v>0.6825</v>
       </c>
       <c r="O50" s="39" t="s">
@@ -4905,7 +4905,7 @@
         <v>44</v>
       </c>
       <c r="B51" s="21" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Rate of IPT initiation from TB compartment  Uninfected, not on IPT and HIV compartment  PLHIV not on ART, CD4&gt;200 for gender Female under policy Community ART + IPT</v>
       </c>
       <c r="C51" s="8" t="s">
@@ -4934,7 +4934,7 @@
         <v>379</v>
       </c>
       <c r="L51" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.6825</v>
       </c>
       <c r="O51" s="39" t="s">
@@ -4952,7 +4952,7 @@
         <v>51</v>
       </c>
       <c r="B52" s="21" t="str">
-        <f t="shared" ref="B52:B83" si="4">CONCATENATE("Rate of IPT initiation from TB compartment ",VLOOKUP(E52,TB_SET,2)," and HIV compartment ",VLOOKUP(G52,HIV_SET,2)," for gender ",VLOOKUP(H52,G_SET,2), " under policy ", VLOOKUP(I52, P_SET,2))</f>
+        <f t="shared" ref="B52:B83" si="5">CONCATENATE("Rate of IPT initiation from TB compartment ",VLOOKUP(E52,TB_SET,2)," and HIV compartment ",VLOOKUP(G52,HIV_SET,2)," for gender ",VLOOKUP(H52,G_SET,2), " under policy ", VLOOKUP(I52, P_SET,2))</f>
         <v>Rate of IPT initiation from TB compartment  LTBI, infected recently (at risk for rapid progression) and HIV compartment  PLHIV not on ART, CD4&gt;200 for gender Male under policy Community ART + IPT</v>
       </c>
       <c r="C52" s="8" t="s">
@@ -4981,7 +4981,7 @@
         <v>400</v>
       </c>
       <c r="L52" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.6825</v>
       </c>
       <c r="O52" s="39" t="s">
@@ -4999,7 +4999,7 @@
         <v>53</v>
       </c>
       <c r="B53" s="21" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>Rate of IPT initiation from TB compartment  LTBI, infected recently (at risk for rapid progression) and HIV compartment  PLHIV not on ART, CD4&gt;200 for gender Female under policy Community ART + IPT</v>
       </c>
       <c r="C53" s="8" t="s">
@@ -5028,7 +5028,7 @@
         <v>403</v>
       </c>
       <c r="L53" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.6825</v>
       </c>
       <c r="O53" s="39" t="s">
@@ -5046,7 +5046,7 @@
         <v>60</v>
       </c>
       <c r="B54" s="21" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>Rate of IPT initiation from TB compartment  LTBI, infected remotely and HIV compartment  PLHIV not on ART, CD4&gt;200 for gender Male under policy Community ART + IPT</v>
       </c>
       <c r="C54" s="8" t="s">
@@ -5075,7 +5075,7 @@
         <v>424</v>
       </c>
       <c r="L54" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.6825</v>
       </c>
       <c r="O54" s="39" t="s">
@@ -5093,7 +5093,7 @@
         <v>61</v>
       </c>
       <c r="B55" s="21" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>Rate of IPT initiation from TB compartment  LTBI, infected remotely and HIV compartment  PLHIV not on ART, CD4&gt;200 for gender Female under policy Community ART + IPT</v>
       </c>
       <c r="C55" s="8" t="s">
@@ -5122,7 +5122,7 @@
         <v>427</v>
       </c>
       <c r="L55" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.6825</v>
       </c>
       <c r="O55" s="39" t="s">
@@ -5140,7 +5140,7 @@
         <v>97</v>
       </c>
       <c r="B56" s="21" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>Rate of IPT initiation from TB compartment  Uninfected, not on IPT and HIV compartment  PLHIV not on ART, CD4≤200 for gender Male under policy Standard (baseline)</v>
       </c>
       <c r="C56" s="8" t="s">
@@ -5185,7 +5185,7 @@
         <v>98</v>
       </c>
       <c r="B57" s="21" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>Rate of IPT initiation from TB compartment  Uninfected, not on IPT and HIV compartment  PLHIV not on ART, CD4≤200 for gender Female under policy Standard (baseline)</v>
       </c>
       <c r="C57" s="8" t="s">
@@ -5230,7 +5230,7 @@
         <v>105</v>
       </c>
       <c r="B58" s="21" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>Rate of IPT initiation from TB compartment  LTBI, infected recently (at risk for rapid progression) and HIV compartment  PLHIV not on ART, CD4≤200 for gender Male under policy Standard (baseline)</v>
       </c>
       <c r="C58" s="8" t="s">
@@ -5275,7 +5275,7 @@
         <v>106</v>
       </c>
       <c r="B59" s="21" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>Rate of IPT initiation from TB compartment  LTBI, infected recently (at risk for rapid progression) and HIV compartment  PLHIV not on ART, CD4≤200 for gender Female under policy Standard (baseline)</v>
       </c>
       <c r="C59" s="8" t="s">
@@ -5320,7 +5320,7 @@
         <v>113</v>
       </c>
       <c r="B60" s="21" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>Rate of IPT initiation from TB compartment  LTBI, infected remotely and HIV compartment  PLHIV not on ART, CD4≤200 for gender Male under policy Standard (baseline)</v>
       </c>
       <c r="C60" s="8" t="s">
@@ -5366,7 +5366,7 @@
         <v>114</v>
       </c>
       <c r="B61" s="21" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>Rate of IPT initiation from TB compartment  LTBI, infected remotely and HIV compartment  PLHIV not on ART, CD4≤200 for gender Female under policy Standard (baseline)</v>
       </c>
       <c r="C61" s="8" t="s">
@@ -5412,7 +5412,7 @@
         <v>72</v>
       </c>
       <c r="B62" s="21" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>Rate of IPT initiation from TB compartment  Uninfected, not on IPT and HIV compartment  PLHIV not on ART, CD4≤200 for gender Male under policy Community ART</v>
       </c>
       <c r="C62" s="8" t="s">
@@ -5459,7 +5459,7 @@
         <v>73</v>
       </c>
       <c r="B63" s="21" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>Rate of IPT initiation from TB compartment  Uninfected, not on IPT and HIV compartment  PLHIV not on ART, CD4≤200 for gender Female under policy Community ART</v>
       </c>
       <c r="C63" s="8" t="s">
@@ -5506,7 +5506,7 @@
         <v>80</v>
       </c>
       <c r="B64" s="21" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>Rate of IPT initiation from TB compartment  LTBI, infected recently (at risk for rapid progression) and HIV compartment  PLHIV not on ART, CD4≤200 for gender Male under policy Community ART</v>
       </c>
       <c r="C64" s="8" t="s">
@@ -5551,7 +5551,7 @@
         <v>81</v>
       </c>
       <c r="B65" s="21" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>Rate of IPT initiation from TB compartment  LTBI, infected recently (at risk for rapid progression) and HIV compartment  PLHIV not on ART, CD4≤200 for gender Female under policy Community ART</v>
       </c>
       <c r="C65" s="8" t="s">
@@ -5596,7 +5596,7 @@
         <v>89</v>
       </c>
       <c r="B66" s="21" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>Rate of IPT initiation from TB compartment  LTBI, infected remotely and HIV compartment  PLHIV not on ART, CD4≤200 for gender Male under policy Community ART</v>
       </c>
       <c r="C66" s="8" t="s">
@@ -5642,7 +5642,7 @@
         <v>90</v>
       </c>
       <c r="B67" s="21" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>Rate of IPT initiation from TB compartment  LTBI, infected remotely and HIV compartment  PLHIV not on ART, CD4≤200 for gender Female under policy Community ART</v>
       </c>
       <c r="C67" s="8" t="s">
@@ -5688,7 +5688,7 @@
         <v>45</v>
       </c>
       <c r="B68" s="21" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>Rate of IPT initiation from TB compartment  Uninfected, not on IPT and HIV compartment  PLHIV not on ART, CD4≤200 for gender Male under policy Community ART + IPT</v>
       </c>
       <c r="C68" s="8" t="s">
@@ -5734,7 +5734,7 @@
         <v>46</v>
       </c>
       <c r="B69" s="21" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>Rate of IPT initiation from TB compartment  Uninfected, not on IPT and HIV compartment  PLHIV not on ART, CD4≤200 for gender Female under policy Community ART + IPT</v>
       </c>
       <c r="C69" s="8" t="s">
@@ -5780,7 +5780,7 @@
         <v>54</v>
       </c>
       <c r="B70" s="21" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>Rate of IPT initiation from TB compartment  LTBI, infected recently (at risk for rapid progression) and HIV compartment  PLHIV not on ART, CD4≤200 for gender Male under policy Community ART + IPT</v>
       </c>
       <c r="C70" s="8" t="s">
@@ -5802,7 +5802,7 @@
         <v>3</v>
       </c>
       <c r="J70" s="9" t="str">
-        <f t="shared" ref="J70:J133" si="5">CONCATENATE(C70, "_", E70, IF(E70&lt;&gt;"",",",""), F70, IF(F70&lt;&gt;"",",",""),  G70, IF(G70&lt;&gt;"",",",""),  H70, IF(I70&lt;&gt;"","(",""), I70, IF(I70&lt;&gt;"",")",""))</f>
+        <f t="shared" ref="J70:J133" si="6">CONCATENATE(C70, "_", E70, IF(E70&lt;&gt;"",",",""), F70, IF(F70&lt;&gt;"",",",""),  G70, IF(G70&lt;&gt;"",",",""),  H70, IF(I70&lt;&gt;"","(",""), I70, IF(I70&lt;&gt;"",")",""))</f>
         <v>kappa_3,3,1(3)</v>
       </c>
       <c r="K70" s="9" t="s">
@@ -5826,7 +5826,7 @@
         <v>55</v>
       </c>
       <c r="B71" s="21" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>Rate of IPT initiation from TB compartment  LTBI, infected recently (at risk for rapid progression) and HIV compartment  PLHIV not on ART, CD4≤200 for gender Female under policy Community ART + IPT</v>
       </c>
       <c r="C71" s="8" t="s">
@@ -5848,7 +5848,7 @@
         <v>3</v>
       </c>
       <c r="J71" s="9" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>kappa_3,3,2(3)</v>
       </c>
       <c r="K71" s="9" t="s">
@@ -5872,7 +5872,7 @@
         <v>62</v>
       </c>
       <c r="B72" s="21" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>Rate of IPT initiation from TB compartment  LTBI, infected remotely and HIV compartment  PLHIV not on ART, CD4≤200 for gender Male under policy Community ART + IPT</v>
       </c>
       <c r="C72" s="8" t="s">
@@ -5894,7 +5894,7 @@
         <v>3</v>
       </c>
       <c r="J72" s="9" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>kappa_4,3,1(3)</v>
       </c>
       <c r="K72" s="9" t="s">
@@ -5918,7 +5918,7 @@
         <v>63</v>
       </c>
       <c r="B73" s="21" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>Rate of IPT initiation from TB compartment  LTBI, infected remotely and HIV compartment  PLHIV not on ART, CD4≤200 for gender Female under policy Community ART + IPT</v>
       </c>
       <c r="C73" s="8" t="s">
@@ -5940,7 +5940,7 @@
         <v>3</v>
       </c>
       <c r="J73" s="9" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>kappa_4,3,2(3)</v>
       </c>
       <c r="K73" s="9" t="s">
@@ -5964,7 +5964,7 @@
         <v>99</v>
       </c>
       <c r="B74" s="21" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>Rate of IPT initiation from TB compartment  Uninfected, not on IPT and HIV compartment  PLHIV and on ART for gender Male under policy Standard (baseline)</v>
       </c>
       <c r="C74" s="8" t="s">
@@ -5986,7 +5986,7 @@
         <v>1</v>
       </c>
       <c r="J74" s="9" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>kappa_1,4,1(1)</v>
       </c>
       <c r="K74" s="9" t="s">
@@ -6008,7 +6008,7 @@
         <v>100</v>
       </c>
       <c r="B75" s="21" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>Rate of IPT initiation from TB compartment  Uninfected, not on IPT and HIV compartment  PLHIV and on ART for gender Female under policy Standard (baseline)</v>
       </c>
       <c r="C75" s="8" t="s">
@@ -6030,7 +6030,7 @@
         <v>1</v>
       </c>
       <c r="J75" s="9" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>kappa_1,4,2(1)</v>
       </c>
       <c r="K75" s="9" t="s">
@@ -6052,7 +6052,7 @@
         <v>107</v>
       </c>
       <c r="B76" s="21" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>Rate of IPT initiation from TB compartment  LTBI, infected recently (at risk for rapid progression) and HIV compartment  PLHIV and on ART for gender Male under policy Standard (baseline)</v>
       </c>
       <c r="C76" s="8" t="s">
@@ -6074,7 +6074,7 @@
         <v>1</v>
       </c>
       <c r="J76" s="9" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>kappa_3,4,1(1)</v>
       </c>
       <c r="K76" s="9" t="s">
@@ -6096,7 +6096,7 @@
         <v>108</v>
       </c>
       <c r="B77" s="21" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>Rate of IPT initiation from TB compartment  LTBI, infected recently (at risk for rapid progression) and HIV compartment  PLHIV and on ART for gender Female under policy Standard (baseline)</v>
       </c>
       <c r="C77" s="8" t="s">
@@ -6118,7 +6118,7 @@
         <v>1</v>
       </c>
       <c r="J77" s="9" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>kappa_3,4,2(1)</v>
       </c>
       <c r="K77" s="9" t="s">
@@ -6140,7 +6140,7 @@
         <v>115</v>
       </c>
       <c r="B78" s="21" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>Rate of IPT initiation from TB compartment  LTBI, infected remotely and HIV compartment  PLHIV and on ART for gender Male under policy Standard (baseline)</v>
       </c>
       <c r="C78" s="8" t="s">
@@ -6162,7 +6162,7 @@
         <v>1</v>
       </c>
       <c r="J78" s="9" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>kappa_4,4,1(1)</v>
       </c>
       <c r="K78" s="9" t="s">
@@ -6186,7 +6186,7 @@
         <v>116</v>
       </c>
       <c r="B79" s="21" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>Rate of IPT initiation from TB compartment  LTBI, infected remotely and HIV compartment  PLHIV and on ART for gender Female under policy Standard (baseline)</v>
       </c>
       <c r="C79" s="8" t="s">
@@ -6208,7 +6208,7 @@
         <v>1</v>
       </c>
       <c r="J79" s="9" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>kappa_4,4,2(1)</v>
       </c>
       <c r="K79" s="9" t="s">
@@ -6232,7 +6232,7 @@
         <v>74</v>
       </c>
       <c r="B80" s="21" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>Rate of IPT initiation from TB compartment  Uninfected, not on IPT and HIV compartment  PLHIV and on ART for gender Male under policy Community ART</v>
       </c>
       <c r="C80" s="8" t="s">
@@ -6254,7 +6254,7 @@
         <v>2</v>
       </c>
       <c r="J80" s="9" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>kappa_1,4,1(2)</v>
       </c>
       <c r="K80" s="9" t="s">
@@ -6278,7 +6278,7 @@
         <v>75</v>
       </c>
       <c r="B81" s="21" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>Rate of IPT initiation from TB compartment  Uninfected, not on IPT and HIV compartment  PLHIV and on ART for gender Female under policy Community ART</v>
       </c>
       <c r="C81" s="8" t="s">
@@ -6300,7 +6300,7 @@
         <v>2</v>
       </c>
       <c r="J81" s="9" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>kappa_1,4,2(2)</v>
       </c>
       <c r="K81" s="9" t="s">
@@ -6324,7 +6324,7 @@
         <v>82</v>
       </c>
       <c r="B82" s="21" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>Rate of IPT initiation from TB compartment  LTBI, infected recently (at risk for rapid progression) and HIV compartment  PLHIV and on ART for gender Male under policy Community ART</v>
       </c>
       <c r="C82" s="8" t="s">
@@ -6346,7 +6346,7 @@
         <v>2</v>
       </c>
       <c r="J82" s="9" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>kappa_3,4,1(2)</v>
       </c>
       <c r="K82" s="9" t="s">
@@ -6370,7 +6370,7 @@
         <v>83</v>
       </c>
       <c r="B83" s="21" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>Rate of IPT initiation from TB compartment  LTBI, infected recently (at risk for rapid progression) and HIV compartment  PLHIV and on ART for gender Female under policy Community ART</v>
       </c>
       <c r="C83" s="8" t="s">
@@ -6392,7 +6392,7 @@
         <v>2</v>
       </c>
       <c r="J83" s="9" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>kappa_3,4,2(2)</v>
       </c>
       <c r="K83" s="9" t="s">
@@ -6416,7 +6416,7 @@
         <v>91</v>
       </c>
       <c r="B84" s="21" t="str">
-        <f t="shared" ref="B84:B91" si="6">CONCATENATE("Rate of IPT initiation from TB compartment ",VLOOKUP(E84,TB_SET,2)," and HIV compartment ",VLOOKUP(G84,HIV_SET,2)," for gender ",VLOOKUP(H84,G_SET,2), " under policy ", VLOOKUP(I84, P_SET,2))</f>
+        <f t="shared" ref="B84:B91" si="7">CONCATENATE("Rate of IPT initiation from TB compartment ",VLOOKUP(E84,TB_SET,2)," and HIV compartment ",VLOOKUP(G84,HIV_SET,2)," for gender ",VLOOKUP(H84,G_SET,2), " under policy ", VLOOKUP(I84, P_SET,2))</f>
         <v>Rate of IPT initiation from TB compartment  LTBI, infected remotely and HIV compartment  PLHIV and on ART for gender Male under policy Community ART</v>
       </c>
       <c r="C84" s="8" t="s">
@@ -6438,7 +6438,7 @@
         <v>2</v>
       </c>
       <c r="J84" s="9" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>kappa_4,4,1(2)</v>
       </c>
       <c r="K84" s="9" t="s">
@@ -6462,7 +6462,7 @@
         <v>92</v>
       </c>
       <c r="B85" s="21" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>Rate of IPT initiation from TB compartment  LTBI, infected remotely and HIV compartment  PLHIV and on ART for gender Female under policy Community ART</v>
       </c>
       <c r="C85" s="8" t="s">
@@ -6484,7 +6484,7 @@
         <v>2</v>
       </c>
       <c r="J85" s="9" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>kappa_4,4,2(2)</v>
       </c>
       <c r="K85" s="9" t="s">
@@ -6508,7 +6508,7 @@
         <v>47</v>
       </c>
       <c r="B86" s="21" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>Rate of IPT initiation from TB compartment  Uninfected, not on IPT and HIV compartment  PLHIV and on ART for gender Male under policy Community ART + IPT</v>
       </c>
       <c r="C86" s="8" t="s">
@@ -6530,7 +6530,7 @@
         <v>3</v>
       </c>
       <c r="J86" s="9" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>kappa_1,4,1(3)</v>
       </c>
       <c r="K86" s="9" t="s">
@@ -6554,7 +6554,7 @@
         <v>48</v>
       </c>
       <c r="B87" s="21" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>Rate of IPT initiation from TB compartment  Uninfected, not on IPT and HIV compartment  PLHIV and on ART for gender Female under policy Community ART + IPT</v>
       </c>
       <c r="C87" s="8" t="s">
@@ -6576,7 +6576,7 @@
         <v>3</v>
       </c>
       <c r="J87" s="9" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>kappa_1,4,2(3)</v>
       </c>
       <c r="K87" s="9" t="s">
@@ -6600,7 +6600,7 @@
         <v>56</v>
       </c>
       <c r="B88" s="21" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>Rate of IPT initiation from TB compartment  LTBI, infected recently (at risk for rapid progression) and HIV compartment  PLHIV and on ART for gender Male under policy Community ART + IPT</v>
       </c>
       <c r="C88" s="8" t="s">
@@ -6622,7 +6622,7 @@
         <v>3</v>
       </c>
       <c r="J88" s="9" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>kappa_3,4,1(3)</v>
       </c>
       <c r="K88" s="9" t="s">
@@ -6646,7 +6646,7 @@
         <v>57</v>
       </c>
       <c r="B89" s="21" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>Rate of IPT initiation from TB compartment  LTBI, infected recently (at risk for rapid progression) and HIV compartment  PLHIV and on ART for gender Female under policy Community ART + IPT</v>
       </c>
       <c r="C89" s="8" t="s">
@@ -6668,7 +6668,7 @@
         <v>3</v>
       </c>
       <c r="J89" s="9" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>kappa_3,4,2(3)</v>
       </c>
       <c r="K89" s="9" t="s">
@@ -6692,7 +6692,7 @@
         <v>64</v>
       </c>
       <c r="B90" s="21" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>Rate of IPT initiation from TB compartment  LTBI, infected remotely and HIV compartment  PLHIV and on ART for gender Male under policy Community ART + IPT</v>
       </c>
       <c r="C90" s="8" t="s">
@@ -6714,7 +6714,7 @@
         <v>3</v>
       </c>
       <c r="J90" s="9" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>kappa_4,4,1(3)</v>
       </c>
       <c r="K90" s="9" t="s">
@@ -6738,7 +6738,7 @@
         <v>65</v>
       </c>
       <c r="B91" s="21" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>Rate of IPT initiation from TB compartment  LTBI, infected remotely and HIV compartment  PLHIV and on ART for gender Female under policy Community ART + IPT</v>
       </c>
       <c r="C91" s="8" t="s">
@@ -6760,7 +6760,7 @@
         <v>3</v>
       </c>
       <c r="J91" s="9" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>kappa_4,4,2(3)</v>
       </c>
       <c r="K91" s="9" t="s">
@@ -6791,7 +6791,7 @@
       </c>
       <c r="E92" s="8"/>
       <c r="J92" s="9" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>omega_</v>
       </c>
       <c r="K92" s="9" t="s">
@@ -6825,7 +6825,7 @@
         <v>34</v>
       </c>
       <c r="J93" s="9" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>pi_34,</v>
       </c>
       <c r="K93" s="9" t="s">
@@ -6859,7 +6859,7 @@
         <v>36</v>
       </c>
       <c r="J94" s="9" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>pi_36,</v>
       </c>
       <c r="K94" s="9" t="s">
@@ -6893,7 +6893,7 @@
         <v>46</v>
       </c>
       <c r="J95" s="9" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>pi_46,</v>
       </c>
       <c r="K95" s="9" t="s">
@@ -6927,7 +6927,7 @@
         <v>56</v>
       </c>
       <c r="J96" s="9" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>pi_56,</v>
       </c>
       <c r="K96" s="9" t="s">
@@ -6939,7 +6939,7 @@
       </c>
       <c r="O96" s="39"/>
       <c r="P96" s="40" t="s">
-        <v>637</v>
+        <v>634</v>
       </c>
       <c r="Q96" s="41" t="s">
         <v>314</v>
@@ -6962,7 +6962,7 @@
         <v>76</v>
       </c>
       <c r="J97" s="9" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>pi_76,</v>
       </c>
       <c r="K97" s="9" t="s">
@@ -6972,16 +6972,16 @@
         <v>8.0000000000000002E-3</v>
       </c>
       <c r="O97" s="9" t="s">
-        <v>637</v>
+        <v>634</v>
       </c>
       <c r="P97" s="40" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
       <c r="Q97" s="10" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="98" spans="1:17" ht="34" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A98" s="22" t="s">
         <v>235</v>
       </c>
@@ -6998,7 +6998,7 @@
         <v>67</v>
       </c>
       <c r="J98" s="9" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>pi_67,</v>
       </c>
       <c r="K98" s="9" t="s">
@@ -7007,11 +7007,9 @@
       <c r="L98" s="23">
         <v>2</v>
       </c>
-      <c r="O98" s="64" t="s">
-        <v>635</v>
-      </c>
+      <c r="O98" s="64"/>
       <c r="P98" s="65" t="s">
-        <v>636</v>
+        <v>633</v>
       </c>
       <c r="Q98" s="41" t="s">
         <v>314</v>
@@ -7032,7 +7030,7 @@
         <v>86</v>
       </c>
       <c r="J99" s="9" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>pi_86,</v>
       </c>
       <c r="K99" s="9" t="s">
@@ -7044,7 +7042,7 @@
       </c>
       <c r="O99" s="39"/>
       <c r="P99" s="40" t="s">
-        <v>637</v>
+        <v>634</v>
       </c>
       <c r="Q99" s="41"/>
     </row>
@@ -7067,7 +7065,7 @@
         <v>1</v>
       </c>
       <c r="J100" s="9" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>theta_1,</v>
       </c>
       <c r="K100" s="9" t="s">
@@ -7077,7 +7075,7 @@
         <v>1</v>
       </c>
       <c r="O100" s="39" t="s">
-        <v>638</v>
+        <v>635</v>
       </c>
       <c r="P100" s="40" t="s">
         <v>311</v>
@@ -7105,7 +7103,7 @@
         <v>2</v>
       </c>
       <c r="J101" s="9" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>theta_2,</v>
       </c>
       <c r="K101" s="9" t="s">
@@ -7115,7 +7113,7 @@
         <v>8</v>
       </c>
       <c r="O101" s="39" t="s">
-        <v>638</v>
+        <v>635</v>
       </c>
       <c r="P101" s="40" t="s">
         <v>311</v>
@@ -7143,7 +7141,7 @@
         <v>3</v>
       </c>
       <c r="J102" s="9" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>theta_3,</v>
       </c>
       <c r="K102" s="9" t="s">
@@ -7153,7 +7151,7 @@
         <v>15</v>
       </c>
       <c r="O102" s="39" t="s">
-        <v>638</v>
+        <v>635</v>
       </c>
       <c r="P102" s="40" t="s">
         <v>311</v>
@@ -7181,7 +7179,7 @@
         <v>4</v>
       </c>
       <c r="J103" s="9" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>theta_4,</v>
       </c>
       <c r="K103" s="9" t="s">
@@ -7191,7 +7189,7 @@
         <v>4</v>
       </c>
       <c r="O103" s="39" t="s">
-        <v>638</v>
+        <v>635</v>
       </c>
       <c r="P103" s="40" t="s">
         <v>29</v>
@@ -7205,7 +7203,7 @@
         <v>315</v>
       </c>
       <c r="B104" s="9" t="str">
-        <f t="shared" ref="B104:B127" si="7">CONCATENATE("Rate of populations moving from HIV compartment ",VLOOKUP(ROUND(G104/10,2),HIV_SET,2)," to ", VLOOKUP(MOD(G104,10),HIV_SET,2), " for gender ", VLOOKUP(H104,G_SET,2), " per year under policy ", VLOOKUP(I104, P_SET,2))</f>
+        <f t="shared" ref="B104:B127" si="8">CONCATENATE("Rate of populations moving from HIV compartment ",VLOOKUP(ROUND(G104/10,2),HIV_SET,2)," to ", VLOOKUP(MOD(G104,10),HIV_SET,2), " for gender ", VLOOKUP(H104,G_SET,2), " per year under policy ", VLOOKUP(I104, P_SET,2))</f>
         <v>Rate of populations moving from HIV compartment  HIV-negative to  PLHIV not on ART, CD4&gt;200 for gender Male per year under policy Standard (baseline)</v>
       </c>
       <c r="C104" s="8" t="s">
@@ -7225,7 +7223,7 @@
         <v>1</v>
       </c>
       <c r="J104" s="9" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>eta_12,1(1)</v>
       </c>
       <c r="K104" s="9" t="s">
@@ -7249,7 +7247,7 @@
         <v>327</v>
       </c>
       <c r="B105" s="9" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>Rate of populations moving from HIV compartment  HIV-negative to  PLHIV not on ART, CD4&gt;200 for gender Female per year under policy Standard (baseline)</v>
       </c>
       <c r="C105" s="8" t="s">
@@ -7269,7 +7267,7 @@
         <v>1</v>
       </c>
       <c r="J105" s="9" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>eta_12,2(1)</v>
       </c>
       <c r="K105" s="9" t="s">
@@ -7293,7 +7291,7 @@
         <v>316</v>
       </c>
       <c r="B106" s="9" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>Rate of populations moving from HIV compartment  HIV-negative to  PLHIV not on ART, CD4&gt;200 for gender Male per year under policy Community ART</v>
       </c>
       <c r="C106" s="8" t="s">
@@ -7313,7 +7311,7 @@
         <v>2</v>
       </c>
       <c r="J106" s="9" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>eta_12,1(2)</v>
       </c>
       <c r="K106" s="9" t="s">
@@ -7337,7 +7335,7 @@
         <v>328</v>
       </c>
       <c r="B107" s="9" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>Rate of populations moving from HIV compartment  HIV-negative to  PLHIV not on ART, CD4&gt;200 for gender Female per year under policy Community ART</v>
       </c>
       <c r="C107" s="8" t="s">
@@ -7357,7 +7355,7 @@
         <v>2</v>
       </c>
       <c r="J107" s="9" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>eta_12,2(2)</v>
       </c>
       <c r="K107" s="9" t="s">
@@ -7381,7 +7379,7 @@
         <v>317</v>
       </c>
       <c r="B108" s="9" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>Rate of populations moving from HIV compartment  HIV-negative to  PLHIV not on ART, CD4&gt;200 for gender Male per year under policy Community ART + IPT</v>
       </c>
       <c r="C108" s="8" t="s">
@@ -7401,7 +7399,7 @@
         <v>3</v>
       </c>
       <c r="J108" s="9" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>eta_12,1(3)</v>
       </c>
       <c r="K108" s="9" t="s">
@@ -7425,7 +7423,7 @@
         <v>329</v>
       </c>
       <c r="B109" s="9" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>Rate of populations moving from HIV compartment  HIV-negative to  PLHIV not on ART, CD4&gt;200 for gender Female per year under policy Community ART + IPT</v>
       </c>
       <c r="C109" s="8" t="s">
@@ -7445,7 +7443,7 @@
         <v>3</v>
       </c>
       <c r="J109" s="9" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>eta_12,2(3)</v>
       </c>
       <c r="K109" s="9" t="s">
@@ -7469,7 +7467,7 @@
         <v>318</v>
       </c>
       <c r="B110" s="9" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>Rate of populations moving from HIV compartment  PLHIV not on ART, CD4&gt;200 to  PLHIV not on ART, CD4≤200 for gender Male per year under policy Standard (baseline)</v>
       </c>
       <c r="C110" s="8" t="s">
@@ -7489,7 +7487,7 @@
         <v>1</v>
       </c>
       <c r="J110" s="9" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>eta_23,1(1)</v>
       </c>
       <c r="K110" s="9" t="s">
@@ -7514,7 +7512,7 @@
         <v>330</v>
       </c>
       <c r="B111" s="9" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>Rate of populations moving from HIV compartment  PLHIV not on ART, CD4&gt;200 to  PLHIV not on ART, CD4≤200 for gender Female per year under policy Standard (baseline)</v>
       </c>
       <c r="C111" s="8" t="s">
@@ -7534,7 +7532,7 @@
         <v>1</v>
       </c>
       <c r="J111" s="9" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>eta_23,2(1)</v>
       </c>
       <c r="K111" s="9" t="s">
@@ -7558,7 +7556,7 @@
         <v>319</v>
       </c>
       <c r="B112" s="9" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>Rate of populations moving from HIV compartment  PLHIV not on ART, CD4&gt;200 to  PLHIV not on ART, CD4≤200 for gender Male per year under policy Community ART</v>
       </c>
       <c r="C112" s="8" t="s">
@@ -7578,7 +7576,7 @@
         <v>2</v>
       </c>
       <c r="J112" s="9" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>eta_23,1(2)</v>
       </c>
       <c r="K112" s="9" t="s">
@@ -7603,7 +7601,7 @@
         <v>331</v>
       </c>
       <c r="B113" s="9" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>Rate of populations moving from HIV compartment  PLHIV not on ART, CD4&gt;200 to  PLHIV not on ART, CD4≤200 for gender Female per year under policy Community ART</v>
       </c>
       <c r="C113" s="8" t="s">
@@ -7623,7 +7621,7 @@
         <v>2</v>
       </c>
       <c r="J113" s="9" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>eta_23,2(2)</v>
       </c>
       <c r="K113" s="9" t="s">
@@ -7647,7 +7645,7 @@
         <v>320</v>
       </c>
       <c r="B114" s="9" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>Rate of populations moving from HIV compartment  PLHIV not on ART, CD4&gt;200 to  PLHIV not on ART, CD4≤200 for gender Male per year under policy Community ART + IPT</v>
       </c>
       <c r="C114" s="8" t="s">
@@ -7667,7 +7665,7 @@
         <v>3</v>
       </c>
       <c r="J114" s="9" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>eta_23,1(3)</v>
       </c>
       <c r="K114" s="9" t="s">
@@ -7692,7 +7690,7 @@
         <v>332</v>
       </c>
       <c r="B115" s="9" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>Rate of populations moving from HIV compartment  PLHIV not on ART, CD4&gt;200 to  PLHIV not on ART, CD4≤200 for gender Female per year under policy Community ART + IPT</v>
       </c>
       <c r="C115" s="8" t="s">
@@ -7712,7 +7710,7 @@
         <v>3</v>
       </c>
       <c r="J115" s="9" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>eta_23,2(3)</v>
       </c>
       <c r="K115" s="9" t="s">
@@ -7736,7 +7734,7 @@
         <v>321</v>
       </c>
       <c r="B116" s="9" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>Rate of populations moving from HIV compartment  PLHIV not on ART, CD4&gt;200 to  PLHIV and on ART for gender Male per year under policy Standard (baseline)</v>
       </c>
       <c r="C116" s="8" t="s">
@@ -7756,7 +7754,7 @@
         <v>1</v>
       </c>
       <c r="J116" s="9" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>eta_24,1(1)</v>
       </c>
       <c r="K116" s="9" t="s">
@@ -7776,7 +7774,7 @@
         <v>333</v>
       </c>
       <c r="B117" s="9" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>Rate of populations moving from HIV compartment  PLHIV not on ART, CD4&gt;200 to  PLHIV and on ART for gender Female per year under policy Standard (baseline)</v>
       </c>
       <c r="C117" s="8" t="s">
@@ -7796,7 +7794,7 @@
         <v>1</v>
       </c>
       <c r="J117" s="9" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>eta_24,2(1)</v>
       </c>
       <c r="K117" s="9" t="s">
@@ -7816,7 +7814,7 @@
         <v>322</v>
       </c>
       <c r="B118" s="9" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>Rate of populations moving from HIV compartment  PLHIV not on ART, CD4&gt;200 to  PLHIV and on ART for gender Male per year under policy Community ART</v>
       </c>
       <c r="C118" s="8" t="s">
@@ -7836,7 +7834,7 @@
         <v>2</v>
       </c>
       <c r="J118" s="9" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>eta_24,1(2)</v>
       </c>
       <c r="K118" s="9" t="s">
@@ -7861,7 +7859,7 @@
         <v>334</v>
       </c>
       <c r="B119" s="9" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>Rate of populations moving from HIV compartment  PLHIV not on ART, CD4&gt;200 to  PLHIV and on ART for gender Female per year under policy Community ART</v>
       </c>
       <c r="C119" s="8" t="s">
@@ -7881,7 +7879,7 @@
         <v>2</v>
       </c>
       <c r="J119" s="9" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>eta_24,2(2)</v>
       </c>
       <c r="K119" s="9" t="s">
@@ -7902,7 +7900,7 @@
         <v>323</v>
       </c>
       <c r="B120" s="9" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>Rate of populations moving from HIV compartment  PLHIV not on ART, CD4&gt;200 to  PLHIV and on ART for gender Male per year under policy Community ART + IPT</v>
       </c>
       <c r="C120" s="8" t="s">
@@ -7922,7 +7920,7 @@
         <v>3</v>
       </c>
       <c r="J120" s="9" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>eta_24,1(3)</v>
       </c>
       <c r="K120" s="9" t="s">
@@ -7947,7 +7945,7 @@
         <v>335</v>
       </c>
       <c r="B121" s="9" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>Rate of populations moving from HIV compartment  PLHIV not on ART, CD4&gt;200 to  PLHIV and on ART for gender Female per year under policy Community ART + IPT</v>
       </c>
       <c r="C121" s="8" t="s">
@@ -7967,7 +7965,7 @@
         <v>3</v>
       </c>
       <c r="J121" s="9" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>eta_24,2(3)</v>
       </c>
       <c r="K121" s="9" t="s">
@@ -7990,7 +7988,7 @@
         <v>324</v>
       </c>
       <c r="B122" s="9" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>Rate of populations moving from HIV compartment  PLHIV not on ART, CD4≤200 to  PLHIV and on ART for gender Male per year under policy Standard (baseline)</v>
       </c>
       <c r="C122" s="8" t="s">
@@ -8010,7 +8008,7 @@
         <v>1</v>
       </c>
       <c r="J122" s="9" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>eta_34,1(1)</v>
       </c>
       <c r="K122" s="9" t="s">
@@ -8030,7 +8028,7 @@
         <v>336</v>
       </c>
       <c r="B123" s="9" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>Rate of populations moving from HIV compartment  PLHIV not on ART, CD4≤200 to  PLHIV and on ART for gender Female per year under policy Standard (baseline)</v>
       </c>
       <c r="C123" s="8" t="s">
@@ -8050,7 +8048,7 @@
         <v>1</v>
       </c>
       <c r="J123" s="9" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>eta_34,2(1)</v>
       </c>
       <c r="K123" s="9" t="s">
@@ -8070,7 +8068,7 @@
         <v>325</v>
       </c>
       <c r="B124" s="9" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>Rate of populations moving from HIV compartment  PLHIV not on ART, CD4≤200 to  PLHIV and on ART for gender Male per year under policy Community ART</v>
       </c>
       <c r="C124" s="8" t="s">
@@ -8090,7 +8088,7 @@
         <v>2</v>
       </c>
       <c r="J124" s="9" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>eta_34,1(2)</v>
       </c>
       <c r="K124" s="9" t="s">
@@ -8113,7 +8111,7 @@
         <v>337</v>
       </c>
       <c r="B125" s="9" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>Rate of populations moving from HIV compartment  PLHIV not on ART, CD4≤200 to  PLHIV and on ART for gender Female per year under policy Community ART</v>
       </c>
       <c r="C125" s="8" t="s">
@@ -8133,7 +8131,7 @@
         <v>2</v>
       </c>
       <c r="J125" s="9" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>eta_34,2(2)</v>
       </c>
       <c r="K125" s="9" t="s">
@@ -8154,7 +8152,7 @@
         <v>326</v>
       </c>
       <c r="B126" s="9" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>Rate of populations moving from HIV compartment  PLHIV not on ART, CD4≤200 to  PLHIV and on ART for gender Male per year under policy Community ART + IPT</v>
       </c>
       <c r="C126" s="8" t="s">
@@ -8174,7 +8172,7 @@
         <v>3</v>
       </c>
       <c r="J126" s="9" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>eta_34,1(3)</v>
       </c>
       <c r="K126" s="9" t="s">
@@ -8199,7 +8197,7 @@
         <v>338</v>
       </c>
       <c r="B127" s="9" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>Rate of populations moving from HIV compartment  PLHIV not on ART, CD4≤200 to  PLHIV and on ART for gender Female per year under policy Community ART + IPT</v>
       </c>
       <c r="C127" s="8" t="s">
@@ -8219,7 +8217,7 @@
         <v>3</v>
       </c>
       <c r="J127" s="9" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>eta_34,2(3)</v>
       </c>
       <c r="K127" s="9" t="s">
@@ -8242,7 +8240,7 @@
         <v>346</v>
       </c>
       <c r="B128" s="9" t="str">
-        <f t="shared" ref="B128:B159" si="8">CONCATENATE("Rate of entry due to aging into HIV compartment ", VLOOKUP(G128, HIV_SET, 2), " and gender compartment ", VLOOKUP(H128, G_SET, 2), ", per year")</f>
+        <f t="shared" ref="B128:B159" si="9">CONCATENATE("Rate of entry due to aging into HIV compartment ", VLOOKUP(G128, HIV_SET, 2), " and gender compartment ", VLOOKUP(H128, G_SET, 2), ", per year")</f>
         <v>Rate of entry due to aging into HIV compartment  HIV-negative and gender compartment Male, per year</v>
       </c>
       <c r="C128" s="8" t="s">
@@ -8264,7 +8262,7 @@
         <v>1</v>
       </c>
       <c r="J128" s="9" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>alpha^in_1,1,1,1</v>
       </c>
       <c r="K128" s="9" t="s">
@@ -8287,7 +8285,7 @@
         <v>347</v>
       </c>
       <c r="B129" s="9" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>Rate of entry due to aging into HIV compartment  HIV-negative and gender compartment Female, per year</v>
       </c>
       <c r="C129" s="8" t="s">
@@ -8309,7 +8307,7 @@
         <v>2</v>
       </c>
       <c r="J129" s="9" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>alpha^in_1,1,1,2</v>
       </c>
       <c r="K129" s="9" t="s">
@@ -8332,7 +8330,7 @@
         <v>346</v>
       </c>
       <c r="B130" s="9" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>Rate of entry due to aging into HIV compartment  HIV-negative and gender compartment Male, per year</v>
       </c>
       <c r="C130" s="8" t="s">
@@ -8354,7 +8352,7 @@
         <v>1</v>
       </c>
       <c r="J130" s="9" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>alpha^in_3,1,1,1</v>
       </c>
       <c r="K130" s="9" t="s">
@@ -8377,7 +8375,7 @@
         <v>347</v>
       </c>
       <c r="B131" s="9" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>Rate of entry due to aging into HIV compartment  HIV-negative and gender compartment Female, per year</v>
       </c>
       <c r="C131" s="8" t="s">
@@ -8399,7 +8397,7 @@
         <v>2</v>
       </c>
       <c r="J131" s="9" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>alpha^in_3,1,1,2</v>
       </c>
       <c r="K131" s="9" t="s">
@@ -8422,7 +8420,7 @@
         <v>346</v>
       </c>
       <c r="B132" s="9" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>Rate of entry due to aging into HIV compartment  HIV-negative and gender compartment Male, per year</v>
       </c>
       <c r="C132" s="8" t="s">
@@ -8444,7 +8442,7 @@
         <v>1</v>
       </c>
       <c r="J132" s="9" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>alpha^in_4,1,1,1</v>
       </c>
       <c r="K132" s="9" t="s">
@@ -8467,7 +8465,7 @@
         <v>347</v>
       </c>
       <c r="B133" s="9" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>Rate of entry due to aging into HIV compartment  HIV-negative and gender compartment Female, per year</v>
       </c>
       <c r="C133" s="8" t="s">
@@ -8489,7 +8487,7 @@
         <v>2</v>
       </c>
       <c r="J133" s="9" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>alpha^in_4,1,1,2</v>
       </c>
       <c r="K133" s="9" t="s">
@@ -8512,7 +8510,7 @@
         <v>346</v>
       </c>
       <c r="B134" s="9" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>Rate of entry due to aging into HIV compartment  HIV-negative and gender compartment Male, per year</v>
       </c>
       <c r="C134" s="8" t="s">
@@ -8534,7 +8532,7 @@
         <v>1</v>
       </c>
       <c r="J134" s="9" t="str">
-        <f t="shared" ref="J134:J197" si="9">CONCATENATE(C134, "_", E134, IF(E134&lt;&gt;"",",",""), F134, IF(F134&lt;&gt;"",",",""),  G134, IF(G134&lt;&gt;"",",",""),  H134, IF(I134&lt;&gt;"","(",""), I134, IF(I134&lt;&gt;"",")",""))</f>
+        <f t="shared" ref="J134:J197" si="10">CONCATENATE(C134, "_", E134, IF(E134&lt;&gt;"",",",""), F134, IF(F134&lt;&gt;"",",",""),  G134, IF(G134&lt;&gt;"",",",""),  H134, IF(I134&lt;&gt;"","(",""), I134, IF(I134&lt;&gt;"",")",""))</f>
         <v>alpha^in_6,1,1,1</v>
       </c>
       <c r="K134" s="9" t="s">
@@ -8557,7 +8555,7 @@
         <v>347</v>
       </c>
       <c r="B135" s="9" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>Rate of entry due to aging into HIV compartment  HIV-negative and gender compartment Female, per year</v>
       </c>
       <c r="C135" s="8" t="s">
@@ -8579,7 +8577,7 @@
         <v>2</v>
       </c>
       <c r="J135" s="9" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>alpha^in_6,1,1,2</v>
       </c>
       <c r="K135" s="9" t="s">
@@ -8602,7 +8600,7 @@
         <v>346</v>
       </c>
       <c r="B136" s="9" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>Rate of entry due to aging into HIV compartment  HIV-negative and gender compartment Male, per year</v>
       </c>
       <c r="C136" s="8" t="s">
@@ -8624,7 +8622,7 @@
         <v>1</v>
       </c>
       <c r="J136" s="9" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>alpha^in_1,2,1,1</v>
       </c>
       <c r="K136" s="9" t="s">
@@ -8647,7 +8645,7 @@
         <v>347</v>
       </c>
       <c r="B137" s="9" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>Rate of entry due to aging into HIV compartment  HIV-negative and gender compartment Female, per year</v>
       </c>
       <c r="C137" s="8" t="s">
@@ -8669,7 +8667,7 @@
         <v>2</v>
       </c>
       <c r="J137" s="9" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>alpha^in_1,2,1,2</v>
       </c>
       <c r="K137" s="9" t="s">
@@ -8692,7 +8690,7 @@
         <v>346</v>
       </c>
       <c r="B138" s="9" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>Rate of entry due to aging into HIV compartment  HIV-negative and gender compartment Male, per year</v>
       </c>
       <c r="C138" s="8" t="s">
@@ -8714,7 +8712,7 @@
         <v>1</v>
       </c>
       <c r="J138" s="9" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>alpha^in_3,2,1,1</v>
       </c>
       <c r="K138" s="9" t="s">
@@ -8737,7 +8735,7 @@
         <v>347</v>
       </c>
       <c r="B139" s="9" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>Rate of entry due to aging into HIV compartment  HIV-negative and gender compartment Female, per year</v>
       </c>
       <c r="C139" s="8" t="s">
@@ -8759,7 +8757,7 @@
         <v>2</v>
       </c>
       <c r="J139" s="9" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>alpha^in_3,2,1,2</v>
       </c>
       <c r="K139" s="9" t="s">
@@ -8782,7 +8780,7 @@
         <v>346</v>
       </c>
       <c r="B140" s="9" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>Rate of entry due to aging into HIV compartment  HIV-negative and gender compartment Male, per year</v>
       </c>
       <c r="C140" s="8" t="s">
@@ -8804,7 +8802,7 @@
         <v>1</v>
       </c>
       <c r="J140" s="9" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>alpha^in_4,2,1,1</v>
       </c>
       <c r="K140" s="9" t="s">
@@ -8827,7 +8825,7 @@
         <v>347</v>
       </c>
       <c r="B141" s="9" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>Rate of entry due to aging into HIV compartment  HIV-negative and gender compartment Female, per year</v>
       </c>
       <c r="C141" s="8" t="s">
@@ -8849,7 +8847,7 @@
         <v>2</v>
       </c>
       <c r="J141" s="9" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>alpha^in_4,2,1,2</v>
       </c>
       <c r="K141" s="9" t="s">
@@ -8872,7 +8870,7 @@
         <v>346</v>
       </c>
       <c r="B142" s="9" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>Rate of entry due to aging into HIV compartment  HIV-negative and gender compartment Male, per year</v>
       </c>
       <c r="C142" s="8" t="s">
@@ -8894,7 +8892,7 @@
         <v>1</v>
       </c>
       <c r="J142" s="9" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>alpha^in_6,2,1,1</v>
       </c>
       <c r="K142" s="9" t="s">
@@ -8917,7 +8915,7 @@
         <v>347</v>
       </c>
       <c r="B143" s="9" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>Rate of entry due to aging into HIV compartment  HIV-negative and gender compartment Female, per year</v>
       </c>
       <c r="C143" s="8" t="s">
@@ -8939,7 +8937,7 @@
         <v>2</v>
       </c>
       <c r="J143" s="9" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>alpha^in_6,2,1,2</v>
       </c>
       <c r="K143" s="9" t="s">
@@ -8962,7 +8960,7 @@
         <v>348</v>
       </c>
       <c r="B144" s="9" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>Rate of entry due to aging into HIV compartment  PLHIV not on ART, CD4&gt;200 and gender compartment Male, per year</v>
       </c>
       <c r="C144" s="8" t="s">
@@ -8984,7 +8982,7 @@
         <v>1</v>
       </c>
       <c r="J144" s="9" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>alpha^in_1,1,2,1</v>
       </c>
       <c r="K144" s="9" t="s">
@@ -9007,7 +9005,7 @@
         <v>349</v>
       </c>
       <c r="B145" s="9" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>Rate of entry due to aging into HIV compartment  PLHIV not on ART, CD4&gt;200 and gender compartment Female, per year</v>
       </c>
       <c r="C145" s="8" t="s">
@@ -9029,7 +9027,7 @@
         <v>2</v>
       </c>
       <c r="J145" s="9" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>alpha^in_1,1,2,2</v>
       </c>
       <c r="K145" s="9" t="s">
@@ -9052,7 +9050,7 @@
         <v>348</v>
       </c>
       <c r="B146" s="9" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>Rate of entry due to aging into HIV compartment  PLHIV not on ART, CD4&gt;200 and gender compartment Male, per year</v>
       </c>
       <c r="C146" s="8" t="s">
@@ -9074,7 +9072,7 @@
         <v>1</v>
       </c>
       <c r="J146" s="9" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>alpha^in_3,1,2,1</v>
       </c>
       <c r="K146" s="9" t="s">
@@ -9097,7 +9095,7 @@
         <v>349</v>
       </c>
       <c r="B147" s="9" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>Rate of entry due to aging into HIV compartment  PLHIV not on ART, CD4&gt;200 and gender compartment Female, per year</v>
       </c>
       <c r="C147" s="8" t="s">
@@ -9119,7 +9117,7 @@
         <v>2</v>
       </c>
       <c r="J147" s="9" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>alpha^in_3,1,2,2</v>
       </c>
       <c r="K147" s="9" t="s">
@@ -9142,7 +9140,7 @@
         <v>348</v>
       </c>
       <c r="B148" s="9" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>Rate of entry due to aging into HIV compartment  PLHIV not on ART, CD4&gt;200 and gender compartment Male, per year</v>
       </c>
       <c r="C148" s="8" t="s">
@@ -9164,7 +9162,7 @@
         <v>1</v>
       </c>
       <c r="J148" s="9" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>alpha^in_4,1,2,1</v>
       </c>
       <c r="K148" s="9" t="s">
@@ -9187,7 +9185,7 @@
         <v>349</v>
       </c>
       <c r="B149" s="9" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>Rate of entry due to aging into HIV compartment  PLHIV not on ART, CD4&gt;200 and gender compartment Female, per year</v>
       </c>
       <c r="C149" s="8" t="s">
@@ -9209,7 +9207,7 @@
         <v>2</v>
       </c>
       <c r="J149" s="9" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>alpha^in_4,1,2,2</v>
       </c>
       <c r="K149" s="9" t="s">
@@ -9232,7 +9230,7 @@
         <v>348</v>
       </c>
       <c r="B150" s="9" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>Rate of entry due to aging into HIV compartment  PLHIV not on ART, CD4&gt;200 and gender compartment Male, per year</v>
       </c>
       <c r="C150" s="8" t="s">
@@ -9254,7 +9252,7 @@
         <v>1</v>
       </c>
       <c r="J150" s="9" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>alpha^in_6,1,2,1</v>
       </c>
       <c r="K150" s="9" t="s">
@@ -9277,7 +9275,7 @@
         <v>349</v>
       </c>
       <c r="B151" s="9" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>Rate of entry due to aging into HIV compartment  PLHIV not on ART, CD4&gt;200 and gender compartment Female, per year</v>
       </c>
       <c r="C151" s="8" t="s">
@@ -9299,7 +9297,7 @@
         <v>2</v>
       </c>
       <c r="J151" s="9" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>alpha^in_6,1,2,2</v>
       </c>
       <c r="K151" s="9" t="s">
@@ -9322,7 +9320,7 @@
         <v>348</v>
       </c>
       <c r="B152" s="9" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>Rate of entry due to aging into HIV compartment  PLHIV not on ART, CD4&gt;200 and gender compartment Male, per year</v>
       </c>
       <c r="C152" s="8" t="s">
@@ -9344,7 +9342,7 @@
         <v>1</v>
       </c>
       <c r="J152" s="9" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>alpha^in_1,2,2,1</v>
       </c>
       <c r="K152" s="9" t="s">
@@ -9367,7 +9365,7 @@
         <v>349</v>
       </c>
       <c r="B153" s="9" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>Rate of entry due to aging into HIV compartment  PLHIV not on ART, CD4&gt;200 and gender compartment Female, per year</v>
       </c>
       <c r="C153" s="8" t="s">
@@ -9389,7 +9387,7 @@
         <v>2</v>
       </c>
       <c r="J153" s="9" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>alpha^in_1,2,2,2</v>
       </c>
       <c r="K153" s="9" t="s">
@@ -9412,7 +9410,7 @@
         <v>348</v>
       </c>
       <c r="B154" s="9" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>Rate of entry due to aging into HIV compartment  PLHIV not on ART, CD4&gt;200 and gender compartment Male, per year</v>
       </c>
       <c r="C154" s="8" t="s">
@@ -9434,7 +9432,7 @@
         <v>1</v>
       </c>
       <c r="J154" s="9" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>alpha^in_3,2,2,1</v>
       </c>
       <c r="K154" s="9" t="s">
@@ -9457,7 +9455,7 @@
         <v>349</v>
       </c>
       <c r="B155" s="9" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>Rate of entry due to aging into HIV compartment  PLHIV not on ART, CD4&gt;200 and gender compartment Female, per year</v>
       </c>
       <c r="C155" s="8" t="s">
@@ -9479,7 +9477,7 @@
         <v>2</v>
       </c>
       <c r="J155" s="9" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>alpha^in_3,2,2,2</v>
       </c>
       <c r="K155" s="9" t="s">
@@ -9502,7 +9500,7 @@
         <v>348</v>
       </c>
       <c r="B156" s="9" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>Rate of entry due to aging into HIV compartment  PLHIV not on ART, CD4&gt;200 and gender compartment Male, per year</v>
       </c>
       <c r="C156" s="8" t="s">
@@ -9524,7 +9522,7 @@
         <v>1</v>
       </c>
       <c r="J156" s="9" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>alpha^in_4,2,2,1</v>
       </c>
       <c r="K156" s="9" t="s">
@@ -9547,7 +9545,7 @@
         <v>349</v>
       </c>
       <c r="B157" s="9" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>Rate of entry due to aging into HIV compartment  PLHIV not on ART, CD4&gt;200 and gender compartment Female, per year</v>
       </c>
       <c r="C157" s="8" t="s">
@@ -9569,7 +9567,7 @@
         <v>2</v>
       </c>
       <c r="J157" s="9" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>alpha^in_4,2,2,2</v>
       </c>
       <c r="K157" s="9" t="s">
@@ -9592,7 +9590,7 @@
         <v>348</v>
       </c>
       <c r="B158" s="9" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>Rate of entry due to aging into HIV compartment  PLHIV not on ART, CD4&gt;200 and gender compartment Male, per year</v>
       </c>
       <c r="C158" s="8" t="s">
@@ -9614,7 +9612,7 @@
         <v>1</v>
       </c>
       <c r="J158" s="9" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>alpha^in_6,2,2,1</v>
       </c>
       <c r="K158" s="9" t="s">
@@ -9637,7 +9635,7 @@
         <v>349</v>
       </c>
       <c r="B159" s="9" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>Rate of entry due to aging into HIV compartment  PLHIV not on ART, CD4&gt;200 and gender compartment Female, per year</v>
       </c>
       <c r="C159" s="8" t="s">
@@ -9659,7 +9657,7 @@
         <v>2</v>
       </c>
       <c r="J159" s="9" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>alpha^in_6,2,2,2</v>
       </c>
       <c r="K159" s="9" t="s">
@@ -9682,7 +9680,7 @@
         <v>137</v>
       </c>
       <c r="B160" s="9" t="str">
-        <f t="shared" ref="B160:B191" si="10">CONCATENATE("Mortality rates from populations in TB compartment ",VLOOKUP(E160,TB_SET,2)," and HIV compartment ",VLOOKUP(G160,HIV_SET,2)," and gender compartment ",VLOOKUP(H160,G_SET,2)," per year")</f>
+        <f t="shared" ref="B160:B191" si="11">CONCATENATE("Mortality rates from populations in TB compartment ",VLOOKUP(E160,TB_SET,2)," and HIV compartment ",VLOOKUP(G160,HIV_SET,2)," and gender compartment ",VLOOKUP(H160,G_SET,2)," per year")</f>
         <v>Mortality rates from populations in TB compartment  Uninfected, not on IPT and HIV compartment  HIV-negative and gender compartment Male per year</v>
       </c>
       <c r="C160" s="8" t="s">
@@ -9701,7 +9699,7 @@
         <v>1</v>
       </c>
       <c r="J160" s="9" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>mu_1,1,1</v>
       </c>
       <c r="K160" s="9" t="s">
@@ -9723,7 +9721,7 @@
         <v>140</v>
       </c>
       <c r="B161" s="9" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>Mortality rates from populations in TB compartment  Uninfected, not on IPT and HIV compartment  HIV-negative and gender compartment Female per year</v>
       </c>
       <c r="C161" s="8" t="s">
@@ -9742,7 +9740,7 @@
         <v>2</v>
       </c>
       <c r="J161" s="9" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>mu_1,1,2</v>
       </c>
       <c r="K161" s="9" t="s">
@@ -9765,7 +9763,7 @@
         <v>147</v>
       </c>
       <c r="B162" s="9" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>Mortality rates from populations in TB compartment  Uninfected, on IPT and HIV compartment  HIV-negative and gender compartment Male per year</v>
       </c>
       <c r="C162" s="8" t="s">
@@ -9784,7 +9782,7 @@
         <v>1</v>
       </c>
       <c r="J162" s="9" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>mu_2,1,1</v>
       </c>
       <c r="K162" s="9" t="s">
@@ -9807,7 +9805,7 @@
         <v>148</v>
       </c>
       <c r="B163" s="9" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>Mortality rates from populations in TB compartment  Uninfected, on IPT and HIV compartment  HIV-negative and gender compartment Female per year</v>
       </c>
       <c r="C163" s="8" t="s">
@@ -9826,7 +9824,7 @@
         <v>2</v>
       </c>
       <c r="J163" s="9" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>mu_2,1,2</v>
       </c>
       <c r="K163" s="9" t="s">
@@ -9849,7 +9847,7 @@
         <v>155</v>
       </c>
       <c r="B164" s="9" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>Mortality rates from populations in TB compartment  LTBI, infected recently (at risk for rapid progression) and HIV compartment  HIV-negative and gender compartment Male per year</v>
       </c>
       <c r="C164" s="8" t="s">
@@ -9868,14 +9866,14 @@
         <v>1</v>
       </c>
       <c r="J164" s="9" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>mu_3,1,1</v>
       </c>
       <c r="K164" s="9" t="s">
         <v>514</v>
       </c>
       <c r="L164" s="11">
-        <f t="shared" ref="L164:L169" si="11">L162</f>
+        <f t="shared" ref="L164:L169" si="12">L162</f>
         <v>3.3E-3</v>
       </c>
       <c r="O164" s="39"/>
@@ -9891,7 +9889,7 @@
         <v>156</v>
       </c>
       <c r="B165" s="9" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>Mortality rates from populations in TB compartment  LTBI, infected recently (at risk for rapid progression) and HIV compartment  HIV-negative and gender compartment Female per year</v>
       </c>
       <c r="C165" s="8" t="s">
@@ -9910,14 +9908,14 @@
         <v>2</v>
       </c>
       <c r="J165" s="9" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>mu_3,1,2</v>
       </c>
       <c r="K165" s="9" t="s">
         <v>515</v>
       </c>
       <c r="L165" s="11">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1.9E-3</v>
       </c>
       <c r="O165" s="39"/>
@@ -9933,7 +9931,7 @@
         <v>163</v>
       </c>
       <c r="B166" s="9" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>Mortality rates from populations in TB compartment  LTBI, infected remotely and HIV compartment  HIV-negative and gender compartment Male per year</v>
       </c>
       <c r="C166" s="8" t="s">
@@ -9952,14 +9950,14 @@
         <v>1</v>
       </c>
       <c r="J166" s="9" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>mu_4,1,1</v>
       </c>
       <c r="K166" s="9" t="s">
         <v>522</v>
       </c>
       <c r="L166" s="11">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>3.3E-3</v>
       </c>
       <c r="O166" s="39"/>
@@ -9975,7 +9973,7 @@
         <v>164</v>
       </c>
       <c r="B167" s="9" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>Mortality rates from populations in TB compartment  LTBI, infected remotely and HIV compartment  HIV-negative and gender compartment Female per year</v>
       </c>
       <c r="C167" s="8" t="s">
@@ -9994,14 +9992,14 @@
         <v>2</v>
       </c>
       <c r="J167" s="9" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>mu_4,1,2</v>
       </c>
       <c r="K167" s="9" t="s">
         <v>523</v>
       </c>
       <c r="L167" s="11">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1.9E-3</v>
       </c>
       <c r="O167" s="39"/>
@@ -10017,7 +10015,7 @@
         <v>171</v>
       </c>
       <c r="B168" s="9" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>Mortality rates from populations in TB compartment  LTBI, on IPT and HIV compartment  HIV-negative and gender compartment Male per year</v>
       </c>
       <c r="C168" s="8" t="s">
@@ -10036,14 +10034,14 @@
         <v>1</v>
       </c>
       <c r="J168" s="9" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>mu_5,1,1</v>
       </c>
       <c r="K168" s="9" t="s">
         <v>530</v>
       </c>
       <c r="L168" s="11">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>3.3E-3</v>
       </c>
       <c r="O168" s="39"/>
@@ -10059,7 +10057,7 @@
         <v>172</v>
       </c>
       <c r="B169" s="9" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>Mortality rates from populations in TB compartment  LTBI, on IPT and HIV compartment  HIV-negative and gender compartment Female per year</v>
       </c>
       <c r="C169" s="8" t="s">
@@ -10078,14 +10076,14 @@
         <v>2</v>
       </c>
       <c r="J169" s="9" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>mu_5,1,2</v>
       </c>
       <c r="K169" s="9" t="s">
         <v>531</v>
       </c>
       <c r="L169" s="11">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1.9E-3</v>
       </c>
       <c r="O169" s="39"/>
@@ -10101,7 +10099,7 @@
         <v>179</v>
       </c>
       <c r="B170" s="9" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>Mortality rates from populations in TB compartment  Active and HIV compartment  HIV-negative and gender compartment Male per year</v>
       </c>
       <c r="C170" s="8" t="s">
@@ -10120,7 +10118,7 @@
         <v>1</v>
       </c>
       <c r="J170" s="9" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>mu_6,1,1</v>
       </c>
       <c r="K170" s="9" t="s">
@@ -10143,7 +10141,7 @@
         <v>180</v>
       </c>
       <c r="B171" s="9" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>Mortality rates from populations in TB compartment  Active and HIV compartment  HIV-negative and gender compartment Female per year</v>
       </c>
       <c r="C171" s="8" t="s">
@@ -10162,7 +10160,7 @@
         <v>2</v>
       </c>
       <c r="J171" s="9" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>mu_6,1,2</v>
       </c>
       <c r="K171" s="9" t="s">
@@ -10185,7 +10183,7 @@
         <v>187</v>
       </c>
       <c r="B172" s="9" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>Mortality rates from populations in TB compartment  Recovered/Treated and HIV compartment  HIV-negative and gender compartment Male per year</v>
       </c>
       <c r="C172" s="8" t="s">
@@ -10204,7 +10202,7 @@
         <v>1</v>
       </c>
       <c r="J172" s="9" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>mu_7,1,1</v>
       </c>
       <c r="K172" s="9" t="s">
@@ -10227,7 +10225,7 @@
         <v>188</v>
       </c>
       <c r="B173" s="9" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>Mortality rates from populations in TB compartment  Recovered/Treated and HIV compartment  HIV-negative and gender compartment Female per year</v>
       </c>
       <c r="C173" s="8" t="s">
@@ -10246,7 +10244,7 @@
         <v>2</v>
       </c>
       <c r="J173" s="9" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>mu_7,1,2</v>
       </c>
       <c r="K173" s="9" t="s">
@@ -10269,7 +10267,7 @@
         <v>195</v>
       </c>
       <c r="B174" s="9" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>Mortality rates from populations in TB compartment  LTBI, after IPT and HIV compartment  HIV-negative and gender compartment Male per year</v>
       </c>
       <c r="C174" s="8" t="s">
@@ -10288,7 +10286,7 @@
         <v>1</v>
       </c>
       <c r="J174" s="9" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>mu_8,1,1</v>
       </c>
       <c r="K174" s="9" t="s">
@@ -10311,7 +10309,7 @@
         <v>196</v>
       </c>
       <c r="B175" s="9" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>Mortality rates from populations in TB compartment  LTBI, after IPT and HIV compartment  HIV-negative and gender compartment Female per year</v>
       </c>
       <c r="C175" s="8" t="s">
@@ -10330,7 +10328,7 @@
         <v>2</v>
       </c>
       <c r="J175" s="9" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>mu_8,1,2</v>
       </c>
       <c r="K175" s="9" t="s">
@@ -10353,7 +10351,7 @@
         <v>141</v>
       </c>
       <c r="B176" s="9" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>Mortality rates from populations in TB compartment  Uninfected, not on IPT and HIV compartment  PLHIV not on ART, CD4&gt;200 and gender compartment Male per year</v>
       </c>
       <c r="C176" s="8" t="s">
@@ -10372,7 +10370,7 @@
         <v>1</v>
       </c>
       <c r="J176" s="9" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>mu_1,2,1</v>
       </c>
       <c r="K176" s="9" t="s">
@@ -10395,7 +10393,7 @@
         <v>142</v>
       </c>
       <c r="B177" s="9" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>Mortality rates from populations in TB compartment  Uninfected, not on IPT and HIV compartment  PLHIV not on ART, CD4&gt;200 and gender compartment Female per year</v>
       </c>
       <c r="C177" s="8" t="s">
@@ -10414,7 +10412,7 @@
         <v>2</v>
       </c>
       <c r="J177" s="9" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>mu_1,2,2</v>
       </c>
       <c r="K177" s="9" t="s">
@@ -10437,7 +10435,7 @@
         <v>149</v>
       </c>
       <c r="B178" s="9" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>Mortality rates from populations in TB compartment  Uninfected, on IPT and HIV compartment  PLHIV not on ART, CD4&gt;200 and gender compartment Male per year</v>
       </c>
       <c r="C178" s="8" t="s">
@@ -10456,7 +10454,7 @@
         <v>1</v>
       </c>
       <c r="J178" s="9" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>mu_2,2,1</v>
       </c>
       <c r="K178" s="9" t="s">
@@ -10479,7 +10477,7 @@
         <v>150</v>
       </c>
       <c r="B179" s="9" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>Mortality rates from populations in TB compartment  Uninfected, on IPT and HIV compartment  PLHIV not on ART, CD4&gt;200 and gender compartment Female per year</v>
       </c>
       <c r="C179" s="8" t="s">
@@ -10498,7 +10496,7 @@
         <v>2</v>
       </c>
       <c r="J179" s="9" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>mu_2,2,2</v>
       </c>
       <c r="K179" s="9" t="s">
@@ -10521,7 +10519,7 @@
         <v>157</v>
       </c>
       <c r="B180" s="9" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>Mortality rates from populations in TB compartment  LTBI, infected recently (at risk for rapid progression) and HIV compartment  PLHIV not on ART, CD4&gt;200 and gender compartment Male per year</v>
       </c>
       <c r="C180" s="8" t="s">
@@ -10540,7 +10538,7 @@
         <v>1</v>
       </c>
       <c r="J180" s="9" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>mu_3,2,1</v>
       </c>
       <c r="K180" s="9" t="s">
@@ -10563,7 +10561,7 @@
         <v>158</v>
       </c>
       <c r="B181" s="9" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>Mortality rates from populations in TB compartment  LTBI, infected recently (at risk for rapid progression) and HIV compartment  PLHIV not on ART, CD4&gt;200 and gender compartment Female per year</v>
       </c>
       <c r="C181" s="8" t="s">
@@ -10582,7 +10580,7 @@
         <v>2</v>
       </c>
       <c r="J181" s="9" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>mu_3,2,2</v>
       </c>
       <c r="K181" s="9" t="s">
@@ -10605,7 +10603,7 @@
         <v>165</v>
       </c>
       <c r="B182" s="9" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>Mortality rates from populations in TB compartment  LTBI, infected remotely and HIV compartment  PLHIV not on ART, CD4&gt;200 and gender compartment Male per year</v>
       </c>
       <c r="C182" s="8" t="s">
@@ -10624,7 +10622,7 @@
         <v>1</v>
       </c>
       <c r="J182" s="9" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>mu_4,2,1</v>
       </c>
       <c r="K182" s="9" t="s">
@@ -10647,7 +10645,7 @@
         <v>166</v>
       </c>
       <c r="B183" s="9" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>Mortality rates from populations in TB compartment  LTBI, infected remotely and HIV compartment  PLHIV not on ART, CD4&gt;200 and gender compartment Female per year</v>
       </c>
       <c r="C183" s="8" t="s">
@@ -10666,14 +10664,14 @@
         <v>2</v>
       </c>
       <c r="J183" s="9" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>mu_4,2,2</v>
       </c>
       <c r="K183" s="9" t="s">
         <v>525</v>
       </c>
       <c r="L183" s="11">
-        <f t="shared" ref="L183:L185" si="12">L177</f>
+        <f t="shared" ref="L183:L185" si="13">L177</f>
         <v>9.4999999999999998E-3</v>
       </c>
       <c r="O183" s="39"/>
@@ -10689,7 +10687,7 @@
         <v>173</v>
       </c>
       <c r="B184" s="9" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>Mortality rates from populations in TB compartment  LTBI, on IPT and HIV compartment  PLHIV not on ART, CD4&gt;200 and gender compartment Male per year</v>
       </c>
       <c r="C184" s="8" t="s">
@@ -10708,14 +10706,14 @@
         <v>1</v>
       </c>
       <c r="J184" s="9" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>mu_5,2,1</v>
       </c>
       <c r="K184" s="9" t="s">
         <v>532</v>
       </c>
       <c r="L184" s="11">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>6.6000000000000003E-2</v>
       </c>
       <c r="O184" s="39"/>
@@ -10731,7 +10729,7 @@
         <v>174</v>
       </c>
       <c r="B185" s="9" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>Mortality rates from populations in TB compartment  LTBI, on IPT and HIV compartment  PLHIV not on ART, CD4&gt;200 and gender compartment Female per year</v>
       </c>
       <c r="C185" s="8" t="s">
@@ -10750,14 +10748,14 @@
         <v>2</v>
       </c>
       <c r="J185" s="9" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>mu_5,2,2</v>
       </c>
       <c r="K185" s="9" t="s">
         <v>533</v>
       </c>
       <c r="L185" s="11">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>3.7999999999999999E-2</v>
       </c>
       <c r="O185" s="39"/>
@@ -10773,7 +10771,7 @@
         <v>181</v>
       </c>
       <c r="B186" s="9" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>Mortality rates from populations in TB compartment  Active and HIV compartment  PLHIV not on ART, CD4&gt;200 and gender compartment Male per year</v>
       </c>
       <c r="C186" s="8" t="s">
@@ -10792,7 +10790,7 @@
         <v>1</v>
       </c>
       <c r="J186" s="9" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>mu_6,2,1</v>
       </c>
       <c r="K186" s="9" t="s">
@@ -10817,7 +10815,7 @@
         <v>182</v>
       </c>
       <c r="B187" s="9" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>Mortality rates from populations in TB compartment  Active and HIV compartment  PLHIV not on ART, CD4&gt;200 and gender compartment Female per year</v>
       </c>
       <c r="C187" s="8" t="s">
@@ -10836,7 +10834,7 @@
         <v>2</v>
       </c>
       <c r="J187" s="9" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>mu_6,2,2</v>
       </c>
       <c r="K187" s="9" t="s">
@@ -10861,7 +10859,7 @@
         <v>189</v>
       </c>
       <c r="B188" s="9" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>Mortality rates from populations in TB compartment  Recovered/Treated and HIV compartment  PLHIV not on ART, CD4&gt;200 and gender compartment Male per year</v>
       </c>
       <c r="C188" s="8" t="s">
@@ -10880,7 +10878,7 @@
         <v>1</v>
       </c>
       <c r="J188" s="9" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>mu_7,2,1</v>
       </c>
       <c r="K188" s="9" t="s">
@@ -10903,7 +10901,7 @@
         <v>190</v>
       </c>
       <c r="B189" s="9" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>Mortality rates from populations in TB compartment  Recovered/Treated and HIV compartment  PLHIV not on ART, CD4&gt;200 and gender compartment Female per year</v>
       </c>
       <c r="C189" s="8" t="s">
@@ -10922,7 +10920,7 @@
         <v>2</v>
       </c>
       <c r="J189" s="9" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>mu_7,2,2</v>
       </c>
       <c r="K189" s="9" t="s">
@@ -10945,7 +10943,7 @@
         <v>197</v>
       </c>
       <c r="B190" s="9" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>Mortality rates from populations in TB compartment  LTBI, after IPT and HIV compartment  PLHIV not on ART, CD4&gt;200 and gender compartment Male per year</v>
       </c>
       <c r="C190" s="8" t="s">
@@ -10964,7 +10962,7 @@
         <v>1</v>
       </c>
       <c r="J190" s="9" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>mu_8,2,1</v>
       </c>
       <c r="K190" s="9" t="s">
@@ -10987,7 +10985,7 @@
         <v>198</v>
       </c>
       <c r="B191" s="9" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>Mortality rates from populations in TB compartment  LTBI, after IPT and HIV compartment  PLHIV not on ART, CD4&gt;200 and gender compartment Female per year</v>
       </c>
       <c r="C191" s="8" t="s">
@@ -11006,7 +11004,7 @@
         <v>2</v>
       </c>
       <c r="J191" s="9" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>mu_8,2,2</v>
       </c>
       <c r="K191" s="9" t="s">
@@ -11029,7 +11027,7 @@
         <v>143</v>
       </c>
       <c r="B192" s="9" t="str">
-        <f t="shared" ref="B192:B223" si="13">CONCATENATE("Mortality rates from populations in TB compartment ",VLOOKUP(E192,TB_SET,2)," and HIV compartment ",VLOOKUP(G192,HIV_SET,2)," and gender compartment ",VLOOKUP(H192,G_SET,2)," per year")</f>
+        <f t="shared" ref="B192:B223" si="14">CONCATENATE("Mortality rates from populations in TB compartment ",VLOOKUP(E192,TB_SET,2)," and HIV compartment ",VLOOKUP(G192,HIV_SET,2)," and gender compartment ",VLOOKUP(H192,G_SET,2)," per year")</f>
         <v>Mortality rates from populations in TB compartment  Uninfected, not on IPT and HIV compartment  PLHIV not on ART, CD4≤200 and gender compartment Male per year</v>
       </c>
       <c r="C192" s="8" t="s">
@@ -11048,7 +11046,7 @@
         <v>1</v>
       </c>
       <c r="J192" s="9" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>mu_1,3,1</v>
       </c>
       <c r="K192" s="9" t="s">
@@ -11071,7 +11069,7 @@
         <v>144</v>
       </c>
       <c r="B193" s="9" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>Mortality rates from populations in TB compartment  Uninfected, not on IPT and HIV compartment  PLHIV not on ART, CD4≤200 and gender compartment Female per year</v>
       </c>
       <c r="C193" s="8" t="s">
@@ -11090,7 +11088,7 @@
         <v>2</v>
       </c>
       <c r="J193" s="9" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>mu_1,3,2</v>
       </c>
       <c r="K193" s="9" t="s">
@@ -11113,7 +11111,7 @@
         <v>151</v>
       </c>
       <c r="B194" s="9" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>Mortality rates from populations in TB compartment  Uninfected, on IPT and HIV compartment  PLHIV not on ART, CD4≤200 and gender compartment Male per year</v>
       </c>
       <c r="C194" s="8" t="s">
@@ -11132,7 +11130,7 @@
         <v>1</v>
       </c>
       <c r="J194" s="9" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>mu_2,3,1</v>
       </c>
       <c r="K194" s="9" t="s">
@@ -11155,7 +11153,7 @@
         <v>152</v>
       </c>
       <c r="B195" s="9" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>Mortality rates from populations in TB compartment  Uninfected, on IPT and HIV compartment  PLHIV not on ART, CD4≤200 and gender compartment Female per year</v>
       </c>
       <c r="C195" s="8" t="s">
@@ -11174,7 +11172,7 @@
         <v>2</v>
       </c>
       <c r="J195" s="9" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>mu_2,3,2</v>
       </c>
       <c r="K195" s="9" t="s">
@@ -11197,7 +11195,7 @@
         <v>159</v>
       </c>
       <c r="B196" s="9" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>Mortality rates from populations in TB compartment  LTBI, infected recently (at risk for rapid progression) and HIV compartment  PLHIV not on ART, CD4≤200 and gender compartment Male per year</v>
       </c>
       <c r="C196" s="8" t="s">
@@ -11216,7 +11214,7 @@
         <v>1</v>
       </c>
       <c r="J196" s="9" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>mu_3,3,1</v>
       </c>
       <c r="K196" s="9" t="s">
@@ -11239,7 +11237,7 @@
         <v>160</v>
       </c>
       <c r="B197" s="9" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>Mortality rates from populations in TB compartment  LTBI, infected recently (at risk for rapid progression) and HIV compartment  PLHIV not on ART, CD4≤200 and gender compartment Female per year</v>
       </c>
       <c r="C197" s="8" t="s">
@@ -11258,7 +11256,7 @@
         <v>2</v>
       </c>
       <c r="J197" s="9" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>mu_3,3,2</v>
       </c>
       <c r="K197" s="9" t="s">
@@ -11281,7 +11279,7 @@
         <v>167</v>
       </c>
       <c r="B198" s="9" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>Mortality rates from populations in TB compartment  LTBI, infected remotely and HIV compartment  PLHIV not on ART, CD4≤200 and gender compartment Male per year</v>
       </c>
       <c r="C198" s="8" t="s">
@@ -11300,7 +11298,7 @@
         <v>1</v>
       </c>
       <c r="J198" s="9" t="str">
-        <f t="shared" ref="J198:J223" si="14">CONCATENATE(C198, "_", E198, IF(E198&lt;&gt;"",",",""), F198, IF(F198&lt;&gt;"",",",""),  G198, IF(G198&lt;&gt;"",",",""),  H198, IF(I198&lt;&gt;"","(",""), I198, IF(I198&lt;&gt;"",")",""))</f>
+        <f t="shared" ref="J198:J223" si="15">CONCATENATE(C198, "_", E198, IF(E198&lt;&gt;"",",",""), F198, IF(F198&lt;&gt;"",",",""),  G198, IF(G198&lt;&gt;"",",",""),  H198, IF(I198&lt;&gt;"","(",""), I198, IF(I198&lt;&gt;"",")",""))</f>
         <v>mu_4,3,1</v>
       </c>
       <c r="K198" s="9" t="s">
@@ -11323,7 +11321,7 @@
         <v>168</v>
       </c>
       <c r="B199" s="9" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>Mortality rates from populations in TB compartment  LTBI, infected remotely and HIV compartment  PLHIV not on ART, CD4≤200 and gender compartment Female per year</v>
       </c>
       <c r="C199" s="8" t="s">
@@ -11342,7 +11340,7 @@
         <v>2</v>
       </c>
       <c r="J199" s="9" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>mu_4,3,2</v>
       </c>
       <c r="K199" s="9" t="s">
@@ -11365,7 +11363,7 @@
         <v>175</v>
       </c>
       <c r="B200" s="9" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>Mortality rates from populations in TB compartment  LTBI, on IPT and HIV compartment  PLHIV not on ART, CD4≤200 and gender compartment Male per year</v>
       </c>
       <c r="C200" s="8" t="s">
@@ -11384,7 +11382,7 @@
         <v>1</v>
       </c>
       <c r="J200" s="9" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>mu_5,3,1</v>
       </c>
       <c r="K200" s="9" t="s">
@@ -11407,7 +11405,7 @@
         <v>176</v>
       </c>
       <c r="B201" s="9" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>Mortality rates from populations in TB compartment  LTBI, on IPT and HIV compartment  PLHIV not on ART, CD4≤200 and gender compartment Female per year</v>
       </c>
       <c r="C201" s="8" t="s">
@@ -11426,7 +11424,7 @@
         <v>2</v>
       </c>
       <c r="J201" s="9" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>mu_5,3,2</v>
       </c>
       <c r="K201" s="9" t="s">
@@ -11449,7 +11447,7 @@
         <v>183</v>
       </c>
       <c r="B202" s="9" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>Mortality rates from populations in TB compartment  Active and HIV compartment  PLHIV not on ART, CD4≤200 and gender compartment Male per year</v>
       </c>
       <c r="C202" s="8" t="s">
@@ -11468,7 +11466,7 @@
         <v>1</v>
       </c>
       <c r="J202" s="9" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>mu_6,3,1</v>
       </c>
       <c r="K202" s="9" t="s">
@@ -11493,7 +11491,7 @@
         <v>184</v>
       </c>
       <c r="B203" s="9" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>Mortality rates from populations in TB compartment  Active and HIV compartment  PLHIV not on ART, CD4≤200 and gender compartment Female per year</v>
       </c>
       <c r="C203" s="8" t="s">
@@ -11512,7 +11510,7 @@
         <v>2</v>
       </c>
       <c r="J203" s="9" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>mu_6,3,2</v>
       </c>
       <c r="K203" s="9" t="s">
@@ -11537,7 +11535,7 @@
         <v>191</v>
       </c>
       <c r="B204" s="9" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>Mortality rates from populations in TB compartment  Recovered/Treated and HIV compartment  PLHIV not on ART, CD4≤200 and gender compartment Male per year</v>
       </c>
       <c r="C204" s="8" t="s">
@@ -11556,7 +11554,7 @@
         <v>1</v>
       </c>
       <c r="J204" s="9" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>mu_7,3,1</v>
       </c>
       <c r="K204" s="9" t="s">
@@ -11579,7 +11577,7 @@
         <v>192</v>
       </c>
       <c r="B205" s="9" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>Mortality rates from populations in TB compartment  Recovered/Treated and HIV compartment  PLHIV not on ART, CD4≤200 and gender compartment Female per year</v>
       </c>
       <c r="C205" s="8" t="s">
@@ -11598,7 +11596,7 @@
         <v>2</v>
       </c>
       <c r="J205" s="9" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>mu_7,3,2</v>
       </c>
       <c r="K205" s="9" t="s">
@@ -11621,7 +11619,7 @@
         <v>199</v>
       </c>
       <c r="B206" s="9" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>Mortality rates from populations in TB compartment  LTBI, after IPT and HIV compartment  PLHIV not on ART, CD4≤200 and gender compartment Male per year</v>
       </c>
       <c r="C206" s="8" t="s">
@@ -11640,7 +11638,7 @@
         <v>1</v>
       </c>
       <c r="J206" s="9" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>mu_8,3,1</v>
       </c>
       <c r="K206" s="9" t="s">
@@ -11663,7 +11661,7 @@
         <v>200</v>
       </c>
       <c r="B207" s="9" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>Mortality rates from populations in TB compartment  LTBI, after IPT and HIV compartment  PLHIV not on ART, CD4≤200 and gender compartment Female per year</v>
       </c>
       <c r="C207" s="8" t="s">
@@ -11682,7 +11680,7 @@
         <v>2</v>
       </c>
       <c r="J207" s="9" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>mu_8,3,2</v>
       </c>
       <c r="K207" s="9" t="s">
@@ -11705,7 +11703,7 @@
         <v>145</v>
       </c>
       <c r="B208" s="9" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>Mortality rates from populations in TB compartment  Uninfected, not on IPT and HIV compartment  PLHIV and on ART and gender compartment Male per year</v>
       </c>
       <c r="C208" s="8" t="s">
@@ -11724,7 +11722,7 @@
         <v>1</v>
       </c>
       <c r="J208" s="9" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>mu_1,4,1</v>
       </c>
       <c r="K208" s="9" t="s">
@@ -11747,7 +11745,7 @@
         <v>146</v>
       </c>
       <c r="B209" s="9" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>Mortality rates from populations in TB compartment  Uninfected, not on IPT and HIV compartment  PLHIV and on ART and gender compartment Female per year</v>
       </c>
       <c r="C209" s="8" t="s">
@@ -11766,7 +11764,7 @@
         <v>2</v>
       </c>
       <c r="J209" s="9" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>mu_1,4,2</v>
       </c>
       <c r="K209" s="9" t="s">
@@ -11789,7 +11787,7 @@
         <v>153</v>
       </c>
       <c r="B210" s="9" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>Mortality rates from populations in TB compartment  Uninfected, on IPT and HIV compartment  PLHIV and on ART and gender compartment Male per year</v>
       </c>
       <c r="C210" s="8" t="s">
@@ -11808,7 +11806,7 @@
         <v>1</v>
       </c>
       <c r="J210" s="9" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>mu_2,4,1</v>
       </c>
       <c r="K210" s="9" t="s">
@@ -11831,7 +11829,7 @@
         <v>154</v>
       </c>
       <c r="B211" s="9" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>Mortality rates from populations in TB compartment  Uninfected, on IPT and HIV compartment  PLHIV and on ART and gender compartment Female per year</v>
       </c>
       <c r="C211" s="8" t="s">
@@ -11850,7 +11848,7 @@
         <v>2</v>
       </c>
       <c r="J211" s="9" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>mu_2,4,2</v>
       </c>
       <c r="K211" s="9" t="s">
@@ -11873,7 +11871,7 @@
         <v>161</v>
       </c>
       <c r="B212" s="9" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>Mortality rates from populations in TB compartment  LTBI, infected recently (at risk for rapid progression) and HIV compartment  PLHIV and on ART and gender compartment Male per year</v>
       </c>
       <c r="C212" s="8" t="s">
@@ -11892,7 +11890,7 @@
         <v>1</v>
       </c>
       <c r="J212" s="9" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>mu_3,4,1</v>
       </c>
       <c r="K212" s="9" t="s">
@@ -11915,7 +11913,7 @@
         <v>162</v>
       </c>
       <c r="B213" s="9" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>Mortality rates from populations in TB compartment  LTBI, infected recently (at risk for rapid progression) and HIV compartment  PLHIV and on ART and gender compartment Female per year</v>
       </c>
       <c r="C213" s="8" t="s">
@@ -11934,7 +11932,7 @@
         <v>2</v>
       </c>
       <c r="J213" s="9" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>mu_3,4,2</v>
       </c>
       <c r="K213" s="9" t="s">
@@ -11957,7 +11955,7 @@
         <v>169</v>
       </c>
       <c r="B214" s="9" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>Mortality rates from populations in TB compartment  LTBI, infected remotely and HIV compartment  PLHIV and on ART and gender compartment Male per year</v>
       </c>
       <c r="C214" s="8" t="s">
@@ -11976,7 +11974,7 @@
         <v>1</v>
       </c>
       <c r="J214" s="9" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>mu_4,4,1</v>
       </c>
       <c r="K214" s="9" t="s">
@@ -11999,7 +11997,7 @@
         <v>170</v>
       </c>
       <c r="B215" s="9" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>Mortality rates from populations in TB compartment  LTBI, infected remotely and HIV compartment  PLHIV and on ART and gender compartment Female per year</v>
       </c>
       <c r="C215" s="8" t="s">
@@ -12018,7 +12016,7 @@
         <v>2</v>
       </c>
       <c r="J215" s="9" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>mu_4,4,2</v>
       </c>
       <c r="K215" s="9" t="s">
@@ -12041,7 +12039,7 @@
         <v>177</v>
       </c>
       <c r="B216" s="9" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>Mortality rates from populations in TB compartment  LTBI, on IPT and HIV compartment  PLHIV and on ART and gender compartment Male per year</v>
       </c>
       <c r="C216" s="8" t="s">
@@ -12060,7 +12058,7 @@
         <v>1</v>
       </c>
       <c r="J216" s="9" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>mu_5,4,1</v>
       </c>
       <c r="K216" s="9" t="s">
@@ -12083,7 +12081,7 @@
         <v>178</v>
       </c>
       <c r="B217" s="9" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>Mortality rates from populations in TB compartment  LTBI, on IPT and HIV compartment  PLHIV and on ART and gender compartment Female per year</v>
       </c>
       <c r="C217" s="8" t="s">
@@ -12102,7 +12100,7 @@
         <v>2</v>
       </c>
       <c r="J217" s="9" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>mu_5,4,2</v>
       </c>
       <c r="K217" s="9" t="s">
@@ -12125,7 +12123,7 @@
         <v>185</v>
       </c>
       <c r="B218" s="9" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>Mortality rates from populations in TB compartment  Active and HIV compartment  PLHIV and on ART and gender compartment Male per year</v>
       </c>
       <c r="C218" s="8" t="s">
@@ -12144,7 +12142,7 @@
         <v>1</v>
       </c>
       <c r="J218" s="9" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>mu_6,4,1</v>
       </c>
       <c r="K218" s="9" t="s">
@@ -12169,7 +12167,7 @@
         <v>186</v>
       </c>
       <c r="B219" s="9" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>Mortality rates from populations in TB compartment  Active and HIV compartment  PLHIV and on ART and gender compartment Female per year</v>
       </c>
       <c r="C219" s="8" t="s">
@@ -12188,7 +12186,7 @@
         <v>2</v>
       </c>
       <c r="J219" s="9" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>mu_6,4,2</v>
       </c>
       <c r="K219" s="9" t="s">
@@ -12213,7 +12211,7 @@
         <v>193</v>
       </c>
       <c r="B220" s="9" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>Mortality rates from populations in TB compartment  Recovered/Treated and HIV compartment  PLHIV and on ART and gender compartment Male per year</v>
       </c>
       <c r="C220" s="8" t="s">
@@ -12232,7 +12230,7 @@
         <v>1</v>
       </c>
       <c r="J220" s="9" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>mu_7,4,1</v>
       </c>
       <c r="K220" s="9" t="s">
@@ -12255,7 +12253,7 @@
         <v>194</v>
       </c>
       <c r="B221" s="9" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>Mortality rates from populations in TB compartment  Recovered/Treated and HIV compartment  PLHIV and on ART and gender compartment Female per year</v>
       </c>
       <c r="C221" s="8" t="s">
@@ -12274,7 +12272,7 @@
         <v>2</v>
       </c>
       <c r="J221" s="9" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>mu_7,4,2</v>
       </c>
       <c r="K221" s="9" t="s">
@@ -12297,7 +12295,7 @@
         <v>201</v>
       </c>
       <c r="B222" s="9" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>Mortality rates from populations in TB compartment  LTBI, after IPT and HIV compartment  PLHIV and on ART and gender compartment Male per year</v>
       </c>
       <c r="C222" s="8" t="s">
@@ -12316,7 +12314,7 @@
         <v>1</v>
       </c>
       <c r="J222" s="9" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>mu_8,4,1</v>
       </c>
       <c r="K222" s="9" t="s">
@@ -12339,7 +12337,7 @@
         <v>202</v>
       </c>
       <c r="B223" s="9" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>Mortality rates from populations in TB compartment  LTBI, after IPT and HIV compartment  PLHIV and on ART and gender compartment Female per year</v>
       </c>
       <c r="C223" s="8" t="s">
@@ -12358,7 +12356,7 @@
         <v>2</v>
       </c>
       <c r="J223" s="9" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>mu_8,4,2</v>
       </c>
       <c r="K223" s="9" t="s">

</xml_diff>